<commit_message>
Added Texture coords and index list.
Coloured in texture on Paint.

Signed-off-by: diggijo <joseph.diggins@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/ComputerGraphics.xlsx
+++ b/ComputerGraphics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph\Documents\College\ComputerGraphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01155E7A-3F88-49F6-BCCB-CF01668BF694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6FB2A0-01E8-44CD-926A-3D81A8631DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30750DBD-9253-4277-820E-7E85B054AA9A}"/>
+    <workbookView xWindow="11856" yWindow="2520" windowWidth="17916" windowHeight="8964" xr2:uid="{30750DBD-9253-4277-820E-7E85B054AA9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Vertices List</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>Texture CoOrds List</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Texture Index List</t>
   </si>
 </sst>
 </file>
@@ -500,24 +509,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,6 +516,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -536,6 +545,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -545,16 +557,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2196,10 +2205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCF257B-ADE3-42C2-8A31-91A658BCB112}">
-  <dimension ref="C1:BI72"/>
+  <dimension ref="C1:BV72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q6" workbookViewId="0">
-      <selection activeCell="BB4" sqref="BB4:BC27"/>
+    <sheetView tabSelected="1" topLeftCell="AP2" workbookViewId="0">
+      <selection activeCell="BP4" sqref="BP4:BU55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,8 +2216,8 @@
     <col min="1" max="96" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:61" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="4:61" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="4:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -2225,7 +2234,7 @@
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
     </row>
-    <row r="3" spans="4:61" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D3">
         <v>0</v>
       </c>
@@ -2249,38 +2258,48 @@
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
       <c r="Y3" s="10"/>
-      <c r="AC3" s="43" t="s">
+      <c r="AC3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="45"/>
-      <c r="AO3" s="43" t="s">
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="38"/>
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="39"/>
+      <c r="AO3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AP3" s="44"/>
-      <c r="AQ3" s="44"/>
-      <c r="AR3" s="44"/>
-      <c r="AS3" s="44"/>
-      <c r="AT3" s="44"/>
-      <c r="AU3" s="44"/>
-      <c r="AV3" s="45"/>
-      <c r="BB3" s="43" t="s">
+      <c r="AP3" s="38"/>
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="38"/>
+      <c r="AS3" s="38"/>
+      <c r="AT3" s="38"/>
+      <c r="AU3" s="38"/>
+      <c r="AV3" s="39"/>
+      <c r="BB3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="BC3" s="44"/>
-      <c r="BD3" s="44"/>
-      <c r="BE3" s="44"/>
-      <c r="BF3" s="44"/>
-      <c r="BG3" s="44"/>
-      <c r="BH3" s="44"/>
-      <c r="BI3" s="45"/>
+      <c r="BC3" s="38"/>
+      <c r="BD3" s="38"/>
+      <c r="BE3" s="38"/>
+      <c r="BF3" s="38"/>
+      <c r="BG3" s="38"/>
+      <c r="BH3" s="38"/>
+      <c r="BI3" s="39"/>
+      <c r="BN3" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="BO3" s="38"/>
+      <c r="BP3" s="38"/>
+      <c r="BQ3" s="38"/>
+      <c r="BR3" s="38"/>
+      <c r="BS3" s="38"/>
+      <c r="BT3" s="38"/>
+      <c r="BU3" s="39"/>
     </row>
-    <row r="4" spans="4:61" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -2302,43 +2321,74 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
-      <c r="AC4" s="40">
+      <c r="AC4" s="53">
         <v>0</v>
       </c>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="42">
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="55">
         <v>-5</v>
       </c>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="42">
+      <c r="AF4" s="55"/>
+      <c r="AG4" s="55">
         <v>5</v>
       </c>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="42">
+      <c r="AH4" s="55"/>
+      <c r="AI4" s="55">
         <v>1</v>
       </c>
-      <c r="AJ4" s="41"/>
-      <c r="AO4" s="40">
+      <c r="AJ4" s="54"/>
+      <c r="AO4" s="53">
         <v>0</v>
       </c>
-      <c r="AP4" s="41"/>
-      <c r="AQ4" s="42">
+      <c r="AP4" s="54"/>
+      <c r="AQ4" s="55">
         <v>1</v>
       </c>
-      <c r="AR4" s="42"/>
-      <c r="AS4" s="42">
+      <c r="AR4" s="55"/>
+      <c r="AS4" s="55">
         <v>0</v>
       </c>
-      <c r="AT4" s="42"/>
-      <c r="AU4" s="42">
+      <c r="AT4" s="55"/>
+      <c r="AU4" s="55">
         <v>2</v>
       </c>
-      <c r="AV4" s="41"/>
+      <c r="AV4" s="54"/>
       <c r="AW4" s="46" t="s">
         <v>4</v>
       </c>
+      <c r="BB4" s="37"/>
+      <c r="BC4" s="39"/>
+      <c r="BD4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE4" s="38"/>
+      <c r="BF4" s="39"/>
+      <c r="BG4" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH4" s="38"/>
+      <c r="BI4" s="39"/>
+      <c r="BN4" s="53">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="54"/>
+      <c r="BP4" s="55">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="55"/>
+      <c r="BR4" s="55">
+        <v>0</v>
+      </c>
+      <c r="BS4" s="55"/>
+      <c r="BT4" s="55">
+        <v>2</v>
+      </c>
+      <c r="BU4" s="54"/>
+      <c r="BV4" s="46" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="4:61" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" s="9"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -2360,41 +2410,72 @@
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
-      <c r="AC5" s="37">
+      <c r="AC5" s="45">
         <v>1</v>
       </c>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="39">
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="40">
         <v>5</v>
       </c>
-      <c r="AF5" s="39"/>
-      <c r="AG5" s="39">
+      <c r="AF5" s="40"/>
+      <c r="AG5" s="40">
         <v>5</v>
       </c>
-      <c r="AH5" s="39"/>
-      <c r="AI5" s="39">
+      <c r="AH5" s="40"/>
+      <c r="AI5" s="40">
         <v>1</v>
       </c>
-      <c r="AJ5" s="38"/>
-      <c r="AO5" s="37">
+      <c r="AJ5" s="41"/>
+      <c r="AO5" s="45">
         <v>1</v>
       </c>
-      <c r="AP5" s="38"/>
-      <c r="AQ5" s="39">
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="40">
         <v>1</v>
       </c>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39">
+      <c r="AR5" s="40"/>
+      <c r="AS5" s="40">
         <v>2</v>
       </c>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="39">
+      <c r="AT5" s="40"/>
+      <c r="AU5" s="40">
         <v>5</v>
       </c>
-      <c r="AV5" s="38"/>
+      <c r="AV5" s="41"/>
       <c r="AW5" s="47"/>
+      <c r="BB5" s="45">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="53">
+        <v>50</v>
+      </c>
+      <c r="BE5" s="55"/>
+      <c r="BF5" s="55"/>
+      <c r="BG5" s="55">
+        <v>100</v>
+      </c>
+      <c r="BH5" s="55"/>
+      <c r="BI5" s="54"/>
+      <c r="BN5" s="45">
+        <v>1</v>
+      </c>
+      <c r="BO5" s="41"/>
+      <c r="BP5" s="40">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="40"/>
+      <c r="BR5" s="40">
+        <v>2</v>
+      </c>
+      <c r="BS5" s="40"/>
+      <c r="BT5" s="40">
+        <v>5</v>
+      </c>
+      <c r="BU5" s="41"/>
+      <c r="BV5" s="47"/>
     </row>
-    <row r="6" spans="4:61" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D6">
         <v>2</v>
       </c>
@@ -2422,41 +2503,72 @@
       <c r="W6" s="10"/>
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
-      <c r="AC6" s="37">
+      <c r="AC6" s="45">
         <v>2</v>
       </c>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="39">
+      <c r="AD6" s="41"/>
+      <c r="AE6" s="40">
         <v>-5</v>
       </c>
-      <c r="AF6" s="39"/>
-      <c r="AG6" s="39">
+      <c r="AF6" s="40"/>
+      <c r="AG6" s="40">
         <v>3</v>
       </c>
-      <c r="AH6" s="39"/>
-      <c r="AI6" s="39">
+      <c r="AH6" s="40"/>
+      <c r="AI6" s="40">
         <v>1</v>
       </c>
-      <c r="AJ6" s="38"/>
-      <c r="AO6" s="37">
+      <c r="AJ6" s="41"/>
+      <c r="AO6" s="45">
         <v>2</v>
       </c>
-      <c r="AP6" s="38"/>
-      <c r="AQ6" s="39">
+      <c r="AP6" s="41"/>
+      <c r="AQ6" s="40">
         <v>4</v>
       </c>
-      <c r="AR6" s="39"/>
-      <c r="AS6" s="39">
+      <c r="AR6" s="40"/>
+      <c r="AS6" s="40">
         <v>3</v>
       </c>
-      <c r="AT6" s="39"/>
-      <c r="AU6" s="39">
+      <c r="AT6" s="40"/>
+      <c r="AU6" s="40">
         <v>10</v>
       </c>
-      <c r="AV6" s="38"/>
+      <c r="AV6" s="41"/>
       <c r="AW6" s="47"/>
+      <c r="BB6" s="45">
+        <v>1</v>
+      </c>
+      <c r="BC6" s="40"/>
+      <c r="BD6" s="45">
+        <v>450</v>
+      </c>
+      <c r="BE6" s="40"/>
+      <c r="BF6" s="40"/>
+      <c r="BG6" s="40">
+        <v>100</v>
+      </c>
+      <c r="BH6" s="40"/>
+      <c r="BI6" s="41"/>
+      <c r="BN6" s="45">
+        <v>2</v>
+      </c>
+      <c r="BO6" s="41"/>
+      <c r="BP6" s="40">
+        <v>4</v>
+      </c>
+      <c r="BQ6" s="40"/>
+      <c r="BR6" s="40">
+        <v>3</v>
+      </c>
+      <c r="BS6" s="40"/>
+      <c r="BT6" s="40">
+        <v>10</v>
+      </c>
+      <c r="BU6" s="41"/>
+      <c r="BV6" s="47"/>
     </row>
-    <row r="7" spans="4:61" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H7" s="10"/>
       <c r="I7" s="15"/>
       <c r="J7" s="13"/>
@@ -2475,81 +2587,143 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
-      <c r="AC7" s="37">
+      <c r="AC7" s="45">
         <v>3</v>
       </c>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="39">
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="40">
         <v>-1</v>
       </c>
-      <c r="AF7" s="39"/>
-      <c r="AG7" s="39">
+      <c r="AF7" s="40"/>
+      <c r="AG7" s="40">
         <v>3</v>
       </c>
-      <c r="AH7" s="39"/>
-      <c r="AI7" s="39">
+      <c r="AH7" s="40"/>
+      <c r="AI7" s="40">
         <v>1</v>
       </c>
-      <c r="AJ7" s="38"/>
-      <c r="AO7" s="37">
+      <c r="AJ7" s="41"/>
+      <c r="AO7" s="45">
         <v>3</v>
       </c>
-      <c r="AP7" s="38"/>
-      <c r="AQ7" s="39">
+      <c r="AP7" s="41"/>
+      <c r="AQ7" s="40">
         <v>4</v>
       </c>
-      <c r="AR7" s="39"/>
-      <c r="AS7" s="39">
+      <c r="AR7" s="40"/>
+      <c r="AS7" s="40">
         <v>10</v>
       </c>
-      <c r="AT7" s="39"/>
-      <c r="AU7" s="39">
+      <c r="AT7" s="40"/>
+      <c r="AU7" s="40">
         <v>11</v>
       </c>
-      <c r="AV7" s="38"/>
+      <c r="AV7" s="41"/>
       <c r="AW7" s="47"/>
+      <c r="BB7" s="45">
+        <v>2</v>
+      </c>
+      <c r="BC7" s="41"/>
+      <c r="BD7" s="45">
+        <v>50</v>
+      </c>
+      <c r="BE7" s="40"/>
+      <c r="BF7" s="40"/>
+      <c r="BG7" s="40">
+        <v>180</v>
+      </c>
+      <c r="BH7" s="40"/>
+      <c r="BI7" s="41"/>
+      <c r="BN7" s="45">
+        <v>3</v>
+      </c>
+      <c r="BO7" s="41"/>
+      <c r="BP7" s="40">
+        <v>4</v>
+      </c>
+      <c r="BQ7" s="40"/>
+      <c r="BR7" s="40">
+        <v>10</v>
+      </c>
+      <c r="BS7" s="40"/>
+      <c r="BT7" s="40">
+        <v>11</v>
+      </c>
+      <c r="BU7" s="41"/>
+      <c r="BV7" s="47"/>
     </row>
-    <row r="8" spans="4:61" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I8" s="16"/>
       <c r="J8" s="6"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
-      <c r="AC8" s="37">
+      <c r="AC8" s="45">
         <v>4</v>
       </c>
-      <c r="AD8" s="38"/>
-      <c r="AE8" s="39">
+      <c r="AD8" s="41"/>
+      <c r="AE8" s="40">
         <v>1</v>
       </c>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="39">
+      <c r="AF8" s="40"/>
+      <c r="AG8" s="40">
         <v>3</v>
       </c>
-      <c r="AH8" s="39"/>
-      <c r="AI8" s="39">
+      <c r="AH8" s="40"/>
+      <c r="AI8" s="40">
         <v>1</v>
       </c>
-      <c r="AJ8" s="38"/>
-      <c r="AO8" s="37">
+      <c r="AJ8" s="41"/>
+      <c r="AO8" s="45">
         <v>4</v>
       </c>
-      <c r="AP8" s="38"/>
-      <c r="AQ8" s="39">
+      <c r="AP8" s="41"/>
+      <c r="AQ8" s="40">
         <v>10</v>
       </c>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="39">
+      <c r="AR8" s="40"/>
+      <c r="AS8" s="40">
         <v>13</v>
       </c>
-      <c r="AT8" s="39"/>
-      <c r="AU8" s="39">
+      <c r="AT8" s="40"/>
+      <c r="AU8" s="40">
         <v>11</v>
       </c>
-      <c r="AV8" s="38"/>
+      <c r="AV8" s="41"/>
       <c r="AW8" s="47"/>
+      <c r="BB8" s="45">
+        <v>3</v>
+      </c>
+      <c r="BC8" s="41"/>
+      <c r="BD8" s="45">
+        <v>210</v>
+      </c>
+      <c r="BE8" s="40"/>
+      <c r="BF8" s="40"/>
+      <c r="BG8" s="40">
+        <v>180</v>
+      </c>
+      <c r="BH8" s="40"/>
+      <c r="BI8" s="41"/>
+      <c r="BN8" s="45">
+        <v>4</v>
+      </c>
+      <c r="BO8" s="41"/>
+      <c r="BP8" s="40">
+        <v>10</v>
+      </c>
+      <c r="BQ8" s="40"/>
+      <c r="BR8" s="40">
+        <v>13</v>
+      </c>
+      <c r="BS8" s="40"/>
+      <c r="BT8" s="40">
+        <v>11</v>
+      </c>
+      <c r="BU8" s="41"/>
+      <c r="BV8" s="47"/>
     </row>
-    <row r="9" spans="4:61" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9">
         <v>6</v>
       </c>
@@ -2558,49 +2732,80 @@
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="6"/>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="45"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
-      <c r="AC9" s="37">
+      <c r="AC9" s="45">
         <v>5</v>
       </c>
-      <c r="AD9" s="38"/>
-      <c r="AE9" s="39">
+      <c r="AD9" s="41"/>
+      <c r="AE9" s="40">
         <v>5</v>
       </c>
-      <c r="AF9" s="39"/>
-      <c r="AG9" s="39">
+      <c r="AF9" s="40"/>
+      <c r="AG9" s="40">
         <v>3</v>
       </c>
-      <c r="AH9" s="39"/>
-      <c r="AI9" s="39">
+      <c r="AH9" s="40"/>
+      <c r="AI9" s="40">
         <v>1</v>
       </c>
-      <c r="AJ9" s="38"/>
-      <c r="AO9" s="37">
+      <c r="AJ9" s="41"/>
+      <c r="AO9" s="45">
         <v>5</v>
       </c>
-      <c r="AP9" s="38"/>
-      <c r="AQ9" s="39">
+      <c r="AP9" s="41"/>
+      <c r="AQ9" s="40">
         <v>10</v>
       </c>
-      <c r="AR9" s="39"/>
-      <c r="AS9" s="39">
+      <c r="AR9" s="40"/>
+      <c r="AS9" s="40">
         <v>9</v>
       </c>
-      <c r="AT9" s="39"/>
-      <c r="AU9" s="39">
+      <c r="AT9" s="40"/>
+      <c r="AU9" s="40">
         <v>12</v>
       </c>
-      <c r="AV9" s="38"/>
+      <c r="AV9" s="41"/>
       <c r="AW9" s="47"/>
+      <c r="BB9" s="45">
+        <v>4</v>
+      </c>
+      <c r="BC9" s="41"/>
+      <c r="BD9" s="45">
+        <v>290</v>
+      </c>
+      <c r="BE9" s="40"/>
+      <c r="BF9" s="40"/>
+      <c r="BG9" s="40">
+        <v>180</v>
+      </c>
+      <c r="BH9" s="40"/>
+      <c r="BI9" s="41"/>
+      <c r="BN9" s="45">
+        <v>5</v>
+      </c>
+      <c r="BO9" s="41"/>
+      <c r="BP9" s="40">
+        <v>10</v>
+      </c>
+      <c r="BQ9" s="40"/>
+      <c r="BR9" s="40">
+        <v>9</v>
+      </c>
+      <c r="BS9" s="40"/>
+      <c r="BT9" s="40">
+        <v>12</v>
+      </c>
+      <c r="BU9" s="41"/>
+      <c r="BV9" s="47"/>
     </row>
-    <row r="10" spans="4:61" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
       <c r="G10" s="16"/>
@@ -2610,41 +2815,72 @@
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
-      <c r="AC10" s="37">
+      <c r="AC10" s="45">
         <v>6</v>
       </c>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="39">
+      <c r="AD10" s="41"/>
+      <c r="AE10" s="40">
         <v>-5</v>
       </c>
-      <c r="AF10" s="39"/>
-      <c r="AG10" s="39">
+      <c r="AF10" s="40"/>
+      <c r="AG10" s="40">
         <v>-1</v>
       </c>
-      <c r="AH10" s="39"/>
-      <c r="AI10" s="39">
+      <c r="AH10" s="40"/>
+      <c r="AI10" s="40">
         <v>1</v>
       </c>
-      <c r="AJ10" s="38"/>
-      <c r="AO10" s="37">
+      <c r="AJ10" s="41"/>
+      <c r="AO10" s="45">
         <v>6</v>
       </c>
-      <c r="AP10" s="38"/>
-      <c r="AQ10" s="39">
+      <c r="AP10" s="41"/>
+      <c r="AQ10" s="40">
         <v>10</v>
       </c>
-      <c r="AR10" s="39"/>
-      <c r="AS10" s="39">
+      <c r="AR10" s="40"/>
+      <c r="AS10" s="40">
         <v>12</v>
       </c>
-      <c r="AT10" s="39"/>
-      <c r="AU10" s="39">
+      <c r="AT10" s="40"/>
+      <c r="AU10" s="40">
         <v>13</v>
       </c>
-      <c r="AV10" s="38"/>
+      <c r="AV10" s="41"/>
       <c r="AW10" s="47"/>
+      <c r="BB10" s="45">
+        <v>5</v>
+      </c>
+      <c r="BC10" s="41"/>
+      <c r="BD10" s="45">
+        <v>450</v>
+      </c>
+      <c r="BE10" s="40"/>
+      <c r="BF10" s="40"/>
+      <c r="BG10" s="40">
+        <v>180</v>
+      </c>
+      <c r="BH10" s="40"/>
+      <c r="BI10" s="41"/>
+      <c r="BN10" s="45">
+        <v>6</v>
+      </c>
+      <c r="BO10" s="41"/>
+      <c r="BP10" s="40">
+        <v>10</v>
+      </c>
+      <c r="BQ10" s="40"/>
+      <c r="BR10" s="40">
+        <v>12</v>
+      </c>
+      <c r="BS10" s="40"/>
+      <c r="BT10" s="40">
+        <v>13</v>
+      </c>
+      <c r="BU10" s="41"/>
+      <c r="BV10" s="47"/>
     </row>
-    <row r="11" spans="4:61" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11">
         <v>8</v>
       </c>
@@ -2663,41 +2899,72 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
-      <c r="AC11" s="37">
+      <c r="AC11" s="45">
         <v>7</v>
       </c>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="39">
+      <c r="AD11" s="41"/>
+      <c r="AE11" s="40">
         <v>-3</v>
       </c>
-      <c r="AF11" s="39"/>
-      <c r="AG11" s="39">
+      <c r="AF11" s="40"/>
+      <c r="AG11" s="40">
         <v>-1</v>
       </c>
-      <c r="AH11" s="39"/>
-      <c r="AI11" s="39">
+      <c r="AH11" s="40"/>
+      <c r="AI11" s="40">
         <v>1</v>
       </c>
-      <c r="AJ11" s="38"/>
-      <c r="AO11" s="37">
+      <c r="AJ11" s="41"/>
+      <c r="AO11" s="45">
         <v>7</v>
       </c>
-      <c r="AP11" s="38"/>
-      <c r="AQ11" s="39">
+      <c r="AP11" s="41"/>
+      <c r="AQ11" s="40">
         <v>9</v>
       </c>
-      <c r="AR11" s="39"/>
-      <c r="AS11" s="39">
+      <c r="AR11" s="40"/>
+      <c r="AS11" s="40">
         <v>8</v>
       </c>
-      <c r="AT11" s="39"/>
-      <c r="AU11" s="39">
+      <c r="AT11" s="40"/>
+      <c r="AU11" s="40">
         <v>12</v>
       </c>
-      <c r="AV11" s="38"/>
+      <c r="AV11" s="41"/>
       <c r="AW11" s="47"/>
+      <c r="BB11" s="45">
+        <v>6</v>
+      </c>
+      <c r="BC11" s="41"/>
+      <c r="BD11" s="45">
+        <v>50</v>
+      </c>
+      <c r="BE11" s="40"/>
+      <c r="BF11" s="40"/>
+      <c r="BG11" s="40">
+        <v>340</v>
+      </c>
+      <c r="BH11" s="40"/>
+      <c r="BI11" s="41"/>
+      <c r="BN11" s="45">
+        <v>7</v>
+      </c>
+      <c r="BO11" s="41"/>
+      <c r="BP11" s="40">
+        <v>9</v>
+      </c>
+      <c r="BQ11" s="40"/>
+      <c r="BR11" s="40">
+        <v>8</v>
+      </c>
+      <c r="BS11" s="40"/>
+      <c r="BT11" s="40">
+        <v>12</v>
+      </c>
+      <c r="BU11" s="41"/>
+      <c r="BV11" s="47"/>
     </row>
-    <row r="12" spans="4:61" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E12" s="23"/>
       <c r="F12" s="24"/>
       <c r="H12" s="26"/>
@@ -2706,41 +2973,72 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
-      <c r="AC12" s="37">
+      <c r="AC12" s="45">
         <v>8</v>
       </c>
-      <c r="AD12" s="38"/>
-      <c r="AE12" s="39">
+      <c r="AD12" s="41"/>
+      <c r="AE12" s="40">
         <v>-5</v>
       </c>
-      <c r="AF12" s="39"/>
-      <c r="AG12" s="39">
+      <c r="AF12" s="40"/>
+      <c r="AG12" s="40">
         <v>-3</v>
       </c>
-      <c r="AH12" s="39"/>
-      <c r="AI12" s="39">
+      <c r="AH12" s="40"/>
+      <c r="AI12" s="40">
         <v>1</v>
       </c>
-      <c r="AJ12" s="38"/>
-      <c r="AO12" s="37">
+      <c r="AJ12" s="41"/>
+      <c r="AO12" s="45">
         <v>8</v>
       </c>
-      <c r="AP12" s="38"/>
-      <c r="AQ12" s="39">
+      <c r="AP12" s="41"/>
+      <c r="AQ12" s="40">
         <v>7</v>
       </c>
-      <c r="AR12" s="39"/>
-      <c r="AS12" s="39">
+      <c r="AR12" s="40"/>
+      <c r="AS12" s="40">
         <v>8</v>
       </c>
-      <c r="AT12" s="39"/>
-      <c r="AU12" s="39">
+      <c r="AT12" s="40"/>
+      <c r="AU12" s="40">
         <v>9</v>
       </c>
-      <c r="AV12" s="38"/>
+      <c r="AV12" s="41"/>
       <c r="AW12" s="47"/>
+      <c r="BB12" s="45">
+        <v>7</v>
+      </c>
+      <c r="BC12" s="41"/>
+      <c r="BD12" s="45">
+        <v>130</v>
+      </c>
+      <c r="BE12" s="40"/>
+      <c r="BF12" s="40"/>
+      <c r="BG12" s="40">
+        <v>340</v>
+      </c>
+      <c r="BH12" s="40"/>
+      <c r="BI12" s="41"/>
+      <c r="BN12" s="45">
+        <v>8</v>
+      </c>
+      <c r="BO12" s="41"/>
+      <c r="BP12" s="40">
+        <v>7</v>
+      </c>
+      <c r="BQ12" s="40"/>
+      <c r="BR12" s="40">
+        <v>8</v>
+      </c>
+      <c r="BS12" s="40"/>
+      <c r="BT12" s="40">
+        <v>9</v>
+      </c>
+      <c r="BU12" s="41"/>
+      <c r="BV12" s="47"/>
     </row>
-    <row r="13" spans="4:61" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F13" s="25"/>
       <c r="G13" s="7"/>
       <c r="H13" s="27"/>
@@ -2748,41 +3046,72 @@
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
-      <c r="AC13" s="37">
+      <c r="AC13" s="45">
         <v>9</v>
       </c>
-      <c r="AD13" s="38"/>
-      <c r="AE13" s="39">
+      <c r="AD13" s="41"/>
+      <c r="AE13" s="40">
         <v>-3</v>
       </c>
-      <c r="AF13" s="39"/>
-      <c r="AG13" s="39">
+      <c r="AF13" s="40"/>
+      <c r="AG13" s="40">
         <v>-3</v>
       </c>
-      <c r="AH13" s="39"/>
-      <c r="AI13" s="39">
+      <c r="AH13" s="40"/>
+      <c r="AI13" s="40">
         <v>1</v>
       </c>
-      <c r="AJ13" s="38"/>
-      <c r="AO13" s="37">
+      <c r="AJ13" s="41"/>
+      <c r="AO13" s="45">
         <v>9</v>
       </c>
-      <c r="AP13" s="38"/>
-      <c r="AQ13" s="39">
+      <c r="AP13" s="41"/>
+      <c r="AQ13" s="40">
         <v>7</v>
       </c>
-      <c r="AR13" s="39"/>
-      <c r="AS13" s="39">
+      <c r="AR13" s="40"/>
+      <c r="AS13" s="40">
         <v>6</v>
       </c>
-      <c r="AT13" s="39"/>
-      <c r="AU13" s="39">
+      <c r="AT13" s="40"/>
+      <c r="AU13" s="40">
         <v>8</v>
       </c>
-      <c r="AV13" s="38"/>
+      <c r="AV13" s="41"/>
       <c r="AW13" s="48"/>
+      <c r="BB13" s="45">
+        <v>8</v>
+      </c>
+      <c r="BC13" s="41"/>
+      <c r="BD13" s="45">
+        <v>50</v>
+      </c>
+      <c r="BE13" s="40"/>
+      <c r="BF13" s="40"/>
+      <c r="BG13" s="40">
+        <v>420</v>
+      </c>
+      <c r="BH13" s="40"/>
+      <c r="BI13" s="41"/>
+      <c r="BN13" s="45">
+        <v>9</v>
+      </c>
+      <c r="BO13" s="41"/>
+      <c r="BP13" s="40">
+        <v>7</v>
+      </c>
+      <c r="BQ13" s="40"/>
+      <c r="BR13" s="40">
+        <v>6</v>
+      </c>
+      <c r="BS13" s="40"/>
+      <c r="BT13" s="40">
+        <v>8</v>
+      </c>
+      <c r="BU13" s="41"/>
+      <c r="BV13" s="48"/>
     </row>
-    <row r="14" spans="4:61" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="F14">
         <v>12</v>
       </c>
@@ -2792,233 +3121,421 @@
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
-      <c r="AC14" s="37">
+      <c r="AC14" s="45">
         <v>10</v>
       </c>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="39">
+      <c r="AD14" s="41"/>
+      <c r="AE14" s="40">
         <v>-1</v>
       </c>
-      <c r="AF14" s="39"/>
-      <c r="AG14" s="39">
+      <c r="AF14" s="40"/>
+      <c r="AG14" s="40">
         <v>-3</v>
       </c>
-      <c r="AH14" s="39"/>
-      <c r="AI14" s="39">
+      <c r="AH14" s="40"/>
+      <c r="AI14" s="40">
         <v>1</v>
       </c>
-      <c r="AJ14" s="38"/>
-      <c r="AO14" s="37">
+      <c r="AJ14" s="41"/>
+      <c r="AO14" s="45">
         <v>10</v>
       </c>
-      <c r="AP14" s="38"/>
-      <c r="AQ14" s="39">
+      <c r="AP14" s="41"/>
+      <c r="AQ14" s="40">
         <v>15</v>
       </c>
-      <c r="AR14" s="39"/>
-      <c r="AS14" s="39">
+      <c r="AR14" s="40"/>
+      <c r="AS14" s="40">
         <v>16</v>
       </c>
-      <c r="AT14" s="39"/>
-      <c r="AU14" s="39">
+      <c r="AT14" s="40"/>
+      <c r="AU14" s="40">
         <v>14</v>
       </c>
-      <c r="AV14" s="38"/>
-      <c r="AW14" s="49" t="s">
+      <c r="AV14" s="41"/>
+      <c r="AW14" s="50" t="s">
         <v>5</v>
       </c>
+      <c r="BB14" s="45">
+        <v>9</v>
+      </c>
+      <c r="BC14" s="41"/>
+      <c r="BD14" s="45">
+        <v>130</v>
+      </c>
+      <c r="BE14" s="40"/>
+      <c r="BF14" s="40"/>
+      <c r="BG14" s="40">
+        <v>420</v>
+      </c>
+      <c r="BH14" s="40"/>
+      <c r="BI14" s="41"/>
+      <c r="BN14" s="45">
+        <v>10</v>
+      </c>
+      <c r="BO14" s="41"/>
+      <c r="BP14" s="40">
+        <v>15</v>
+      </c>
+      <c r="BQ14" s="40"/>
+      <c r="BR14" s="40">
+        <v>16</v>
+      </c>
+      <c r="BS14" s="40"/>
+      <c r="BT14" s="40">
+        <v>14</v>
+      </c>
+      <c r="BU14" s="41"/>
+      <c r="BV14" s="50" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="15" spans="4:61" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
-      <c r="AC15" s="37">
+      <c r="AC15" s="45">
         <v>11</v>
       </c>
-      <c r="AD15" s="38"/>
-      <c r="AE15" s="39">
+      <c r="AD15" s="41"/>
+      <c r="AE15" s="40">
         <v>1</v>
       </c>
-      <c r="AF15" s="39"/>
-      <c r="AG15" s="39">
+      <c r="AF15" s="40"/>
+      <c r="AG15" s="40">
         <v>-3</v>
       </c>
-      <c r="AH15" s="39"/>
-      <c r="AI15" s="39">
+      <c r="AH15" s="40"/>
+      <c r="AI15" s="40">
         <v>1</v>
       </c>
-      <c r="AJ15" s="38"/>
-      <c r="AO15" s="37">
+      <c r="AJ15" s="41"/>
+      <c r="AO15" s="45">
         <v>11</v>
       </c>
-      <c r="AP15" s="38"/>
-      <c r="AQ15" s="39">
+      <c r="AP15" s="41"/>
+      <c r="AQ15" s="40">
         <v>15</v>
       </c>
-      <c r="AR15" s="39"/>
-      <c r="AS15" s="39">
+      <c r="AR15" s="40"/>
+      <c r="AS15" s="40">
         <v>19</v>
       </c>
-      <c r="AT15" s="39"/>
-      <c r="AU15" s="39">
+      <c r="AT15" s="40"/>
+      <c r="AU15" s="40">
         <v>16</v>
       </c>
-      <c r="AV15" s="38"/>
-      <c r="AW15" s="50"/>
+      <c r="AV15" s="41"/>
+      <c r="AW15" s="51"/>
+      <c r="BB15" s="45">
+        <v>10</v>
+      </c>
+      <c r="BC15" s="41"/>
+      <c r="BD15" s="45">
+        <v>210</v>
+      </c>
+      <c r="BE15" s="40"/>
+      <c r="BF15" s="40"/>
+      <c r="BG15" s="40">
+        <v>420</v>
+      </c>
+      <c r="BH15" s="40"/>
+      <c r="BI15" s="41"/>
+      <c r="BN15" s="45">
+        <v>11</v>
+      </c>
+      <c r="BO15" s="41"/>
+      <c r="BP15" s="40">
+        <v>15</v>
+      </c>
+      <c r="BQ15" s="40"/>
+      <c r="BR15" s="40">
+        <v>19</v>
+      </c>
+      <c r="BS15" s="40"/>
+      <c r="BT15" s="40">
+        <v>16</v>
+      </c>
+      <c r="BU15" s="41"/>
+      <c r="BV15" s="51"/>
     </row>
-    <row r="16" spans="4:61" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
-      <c r="AC16" s="37">
+      <c r="AC16" s="45">
         <v>12</v>
       </c>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="39">
+      <c r="AD16" s="41"/>
+      <c r="AE16" s="40">
         <v>-3</v>
       </c>
-      <c r="AF16" s="39"/>
-      <c r="AG16" s="39">
+      <c r="AF16" s="40"/>
+      <c r="AG16" s="40">
         <v>-5</v>
       </c>
-      <c r="AH16" s="39"/>
-      <c r="AI16" s="39">
+      <c r="AH16" s="40"/>
+      <c r="AI16" s="40">
         <v>1</v>
       </c>
-      <c r="AJ16" s="38"/>
-      <c r="AO16" s="37">
+      <c r="AJ16" s="41"/>
+      <c r="AO16" s="45">
         <v>12</v>
       </c>
-      <c r="AP16" s="38"/>
-      <c r="AQ16" s="39">
+      <c r="AP16" s="41"/>
+      <c r="AQ16" s="40">
         <v>18</v>
       </c>
-      <c r="AR16" s="39"/>
-      <c r="AS16" s="39">
+      <c r="AR16" s="40"/>
+      <c r="AS16" s="40">
         <v>24</v>
       </c>
-      <c r="AT16" s="39"/>
-      <c r="AU16" s="39">
+      <c r="AT16" s="40"/>
+      <c r="AU16" s="40">
         <v>17</v>
       </c>
-      <c r="AV16" s="38"/>
-      <c r="AW16" s="50"/>
+      <c r="AV16" s="41"/>
+      <c r="AW16" s="51"/>
+      <c r="BB16" s="45">
+        <v>11</v>
+      </c>
+      <c r="BC16" s="41"/>
+      <c r="BD16" s="45">
+        <v>290</v>
+      </c>
+      <c r="BE16" s="40"/>
+      <c r="BF16" s="40"/>
+      <c r="BG16" s="40">
+        <v>420</v>
+      </c>
+      <c r="BH16" s="40"/>
+      <c r="BI16" s="41"/>
+      <c r="BN16" s="45">
+        <v>12</v>
+      </c>
+      <c r="BO16" s="41"/>
+      <c r="BP16" s="40">
+        <v>18</v>
+      </c>
+      <c r="BQ16" s="40"/>
+      <c r="BR16" s="40">
+        <v>24</v>
+      </c>
+      <c r="BS16" s="40"/>
+      <c r="BT16" s="40">
+        <v>17</v>
+      </c>
+      <c r="BU16" s="41"/>
+      <c r="BV16" s="51"/>
     </row>
-    <row r="17" spans="3:49" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
-      <c r="AC17" s="37">
+      <c r="AC17" s="45">
         <v>13</v>
       </c>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="37">
+      <c r="AD17" s="41"/>
+      <c r="AE17" s="45">
         <v>-1</v>
       </c>
-      <c r="AF17" s="39"/>
-      <c r="AG17" s="39">
+      <c r="AF17" s="40"/>
+      <c r="AG17" s="40">
         <v>-5</v>
       </c>
-      <c r="AH17" s="39"/>
-      <c r="AI17" s="39">
+      <c r="AH17" s="40"/>
+      <c r="AI17" s="40">
         <v>1</v>
       </c>
-      <c r="AJ17" s="38"/>
-      <c r="AO17" s="37">
+      <c r="AJ17" s="41"/>
+      <c r="AO17" s="45">
         <v>13</v>
       </c>
-      <c r="AP17" s="38"/>
-      <c r="AQ17" s="39">
+      <c r="AP17" s="41"/>
+      <c r="AQ17" s="40">
         <v>18</v>
       </c>
-      <c r="AR17" s="39"/>
-      <c r="AS17" s="39">
+      <c r="AR17" s="40"/>
+      <c r="AS17" s="40">
         <v>25</v>
       </c>
-      <c r="AT17" s="39"/>
-      <c r="AU17" s="39">
+      <c r="AT17" s="40"/>
+      <c r="AU17" s="40">
         <v>24</v>
       </c>
-      <c r="AV17" s="38"/>
-      <c r="AW17" s="50"/>
+      <c r="AV17" s="41"/>
+      <c r="AW17" s="51"/>
+      <c r="BB17" s="45">
+        <v>12</v>
+      </c>
+      <c r="BC17" s="41"/>
+      <c r="BD17" s="45">
+        <v>130</v>
+      </c>
+      <c r="BE17" s="40"/>
+      <c r="BF17" s="40"/>
+      <c r="BG17" s="40">
+        <v>500</v>
+      </c>
+      <c r="BH17" s="40"/>
+      <c r="BI17" s="41"/>
+      <c r="BN17" s="45">
+        <v>13</v>
+      </c>
+      <c r="BO17" s="41"/>
+      <c r="BP17" s="40">
+        <v>18</v>
+      </c>
+      <c r="BQ17" s="40"/>
+      <c r="BR17" s="40">
+        <v>25</v>
+      </c>
+      <c r="BS17" s="40"/>
+      <c r="BT17" s="40">
+        <v>24</v>
+      </c>
+      <c r="BU17" s="41"/>
+      <c r="BV17" s="51"/>
     </row>
-    <row r="18" spans="3:49" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AC18" s="37">
+    <row r="18" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC18" s="45">
         <v>14</v>
       </c>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="39">
+      <c r="AD18" s="41"/>
+      <c r="AE18" s="40">
         <v>-5</v>
       </c>
-      <c r="AF18" s="39"/>
-      <c r="AG18" s="39">
+      <c r="AF18" s="40"/>
+      <c r="AG18" s="40">
         <v>5</v>
       </c>
-      <c r="AH18" s="39"/>
-      <c r="AI18" s="39">
+      <c r="AH18" s="40"/>
+      <c r="AI18" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ18" s="38"/>
-      <c r="AO18" s="37">
+      <c r="AJ18" s="41"/>
+      <c r="AO18" s="45">
         <v>14</v>
       </c>
-      <c r="AP18" s="38"/>
-      <c r="AQ18" s="39">
+      <c r="AP18" s="41"/>
+      <c r="AQ18" s="40">
         <v>24</v>
       </c>
-      <c r="AR18" s="39"/>
-      <c r="AS18" s="39">
+      <c r="AR18" s="40"/>
+      <c r="AS18" s="40">
         <v>25</v>
       </c>
-      <c r="AT18" s="39"/>
-      <c r="AU18" s="39">
+      <c r="AT18" s="40"/>
+      <c r="AU18" s="40">
         <v>27</v>
       </c>
-      <c r="AV18" s="38"/>
-      <c r="AW18" s="50"/>
+      <c r="AV18" s="41"/>
+      <c r="AW18" s="51"/>
+      <c r="BB18" s="45">
+        <v>13</v>
+      </c>
+      <c r="BC18" s="41"/>
+      <c r="BD18" s="45">
+        <v>210</v>
+      </c>
+      <c r="BE18" s="40"/>
+      <c r="BF18" s="40"/>
+      <c r="BG18" s="40">
+        <v>500</v>
+      </c>
+      <c r="BH18" s="40"/>
+      <c r="BI18" s="41"/>
+      <c r="BN18" s="45">
+        <v>14</v>
+      </c>
+      <c r="BO18" s="41"/>
+      <c r="BP18" s="40">
+        <v>24</v>
+      </c>
+      <c r="BQ18" s="40"/>
+      <c r="BR18" s="40">
+        <v>25</v>
+      </c>
+      <c r="BS18" s="40"/>
+      <c r="BT18" s="40">
+        <v>27</v>
+      </c>
+      <c r="BU18" s="41"/>
+      <c r="BV18" s="51"/>
     </row>
-    <row r="19" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D19">
         <v>15</v>
       </c>
       <c r="O19">
         <v>14</v>
       </c>
-      <c r="AC19" s="37">
+      <c r="AC19" s="45">
         <v>15</v>
       </c>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="39">
+      <c r="AD19" s="41"/>
+      <c r="AE19" s="40">
         <v>5</v>
       </c>
-      <c r="AF19" s="39"/>
-      <c r="AG19" s="39">
+      <c r="AF19" s="40"/>
+      <c r="AG19" s="40">
         <v>5</v>
       </c>
-      <c r="AH19" s="39"/>
-      <c r="AI19" s="39">
+      <c r="AH19" s="40"/>
+      <c r="AI19" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ19" s="38"/>
-      <c r="AO19" s="37">
+      <c r="AJ19" s="41"/>
+      <c r="AO19" s="45">
         <v>15</v>
       </c>
-      <c r="AP19" s="38"/>
-      <c r="AQ19" s="39">
+      <c r="AP19" s="41"/>
+      <c r="AQ19" s="40">
         <v>24</v>
       </c>
-      <c r="AR19" s="39"/>
-      <c r="AS19" s="39">
+      <c r="AR19" s="40"/>
+      <c r="AS19" s="40">
         <v>27</v>
       </c>
-      <c r="AT19" s="39"/>
-      <c r="AU19" s="39">
+      <c r="AT19" s="40"/>
+      <c r="AU19" s="40">
         <v>26</v>
       </c>
-      <c r="AV19" s="38"/>
-      <c r="AW19" s="50"/>
+      <c r="AV19" s="41"/>
+      <c r="AW19" s="51"/>
+      <c r="BB19" s="45">
+        <v>14</v>
+      </c>
+      <c r="BC19" s="41"/>
+      <c r="BD19" s="45">
+        <v>850</v>
+      </c>
+      <c r="BE19" s="40"/>
+      <c r="BF19" s="40"/>
+      <c r="BG19" s="40">
+        <v>500</v>
+      </c>
+      <c r="BH19" s="40"/>
+      <c r="BI19" s="41"/>
+      <c r="BN19" s="45">
+        <v>15</v>
+      </c>
+      <c r="BO19" s="41"/>
+      <c r="BP19" s="40">
+        <v>24</v>
+      </c>
+      <c r="BQ19" s="40"/>
+      <c r="BR19" s="40">
+        <v>27</v>
+      </c>
+      <c r="BS19" s="40"/>
+      <c r="BT19" s="40">
+        <v>26</v>
+      </c>
+      <c r="BU19" s="41"/>
+      <c r="BV19" s="51"/>
     </row>
-    <row r="20" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3029,41 +3546,72 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
       <c r="N20" s="17"/>
-      <c r="AC20" s="37">
+      <c r="AC20" s="45">
         <v>16</v>
       </c>
-      <c r="AD20" s="38"/>
-      <c r="AE20" s="39">
+      <c r="AD20" s="41"/>
+      <c r="AE20" s="40">
         <v>-5</v>
       </c>
-      <c r="AF20" s="39"/>
-      <c r="AG20" s="39">
+      <c r="AF20" s="40"/>
+      <c r="AG20" s="40">
         <v>3</v>
       </c>
-      <c r="AH20" s="39"/>
-      <c r="AI20" s="39">
+      <c r="AH20" s="40"/>
+      <c r="AI20" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ20" s="38"/>
-      <c r="AO20" s="37">
+      <c r="AJ20" s="41"/>
+      <c r="AO20" s="45">
         <v>16</v>
       </c>
-      <c r="AP20" s="38"/>
-      <c r="AQ20" s="39">
+      <c r="AP20" s="41"/>
+      <c r="AQ20" s="40">
         <v>24</v>
       </c>
-      <c r="AR20" s="39"/>
-      <c r="AS20" s="39">
+      <c r="AR20" s="40"/>
+      <c r="AS20" s="40">
         <v>26</v>
       </c>
-      <c r="AT20" s="39"/>
-      <c r="AU20" s="39">
+      <c r="AT20" s="40"/>
+      <c r="AU20" s="40">
         <v>23</v>
       </c>
-      <c r="AV20" s="38"/>
-      <c r="AW20" s="50"/>
+      <c r="AV20" s="41"/>
+      <c r="AW20" s="51"/>
+      <c r="BB20" s="45">
+        <v>15</v>
+      </c>
+      <c r="BC20" s="41"/>
+      <c r="BD20" s="45">
+        <v>450</v>
+      </c>
+      <c r="BE20" s="40"/>
+      <c r="BF20" s="40"/>
+      <c r="BG20" s="40">
+        <v>500</v>
+      </c>
+      <c r="BH20" s="40"/>
+      <c r="BI20" s="41"/>
+      <c r="BN20" s="45">
+        <v>16</v>
+      </c>
+      <c r="BO20" s="41"/>
+      <c r="BP20" s="40">
+        <v>24</v>
+      </c>
+      <c r="BQ20" s="40"/>
+      <c r="BR20" s="40">
+        <v>26</v>
+      </c>
+      <c r="BS20" s="40"/>
+      <c r="BT20" s="40">
+        <v>23</v>
+      </c>
+      <c r="BU20" s="41"/>
+      <c r="BV20" s="51"/>
     </row>
-    <row r="21" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -3074,41 +3622,72 @@
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
       <c r="N21" s="12"/>
-      <c r="AC21" s="37">
+      <c r="AC21" s="45">
         <v>17</v>
       </c>
-      <c r="AD21" s="38"/>
-      <c r="AE21" s="39">
+      <c r="AD21" s="41"/>
+      <c r="AE21" s="40">
         <v>-1</v>
       </c>
-      <c r="AF21" s="39"/>
-      <c r="AG21" s="39">
+      <c r="AF21" s="40"/>
+      <c r="AG21" s="40">
         <v>3</v>
       </c>
-      <c r="AH21" s="39"/>
-      <c r="AI21" s="39">
+      <c r="AH21" s="40"/>
+      <c r="AI21" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ21" s="38"/>
-      <c r="AO21" s="37">
+      <c r="AJ21" s="41"/>
+      <c r="AO21" s="45">
         <v>17</v>
       </c>
-      <c r="AP21" s="38"/>
-      <c r="AQ21" s="37">
+      <c r="AP21" s="41"/>
+      <c r="AQ21" s="45">
         <v>23</v>
       </c>
-      <c r="AR21" s="39"/>
-      <c r="AS21" s="39">
+      <c r="AR21" s="40"/>
+      <c r="AS21" s="40">
         <v>26</v>
       </c>
-      <c r="AT21" s="39"/>
-      <c r="AU21" s="39">
+      <c r="AT21" s="40"/>
+      <c r="AU21" s="40">
         <v>22</v>
       </c>
-      <c r="AV21" s="38"/>
-      <c r="AW21" s="50"/>
+      <c r="AV21" s="41"/>
+      <c r="AW21" s="51"/>
+      <c r="BB21" s="45">
+        <v>16</v>
+      </c>
+      <c r="BC21" s="41"/>
+      <c r="BD21" s="45">
+        <v>850</v>
+      </c>
+      <c r="BE21" s="40"/>
+      <c r="BF21" s="40"/>
+      <c r="BG21" s="40">
+        <v>580</v>
+      </c>
+      <c r="BH21" s="40"/>
+      <c r="BI21" s="41"/>
+      <c r="BN21" s="45">
+        <v>17</v>
+      </c>
+      <c r="BO21" s="41"/>
+      <c r="BP21" s="45">
+        <v>23</v>
+      </c>
+      <c r="BQ21" s="40"/>
+      <c r="BR21" s="40">
+        <v>26</v>
+      </c>
+      <c r="BS21" s="40"/>
+      <c r="BT21" s="40">
+        <v>22</v>
+      </c>
+      <c r="BU21" s="41"/>
+      <c r="BV21" s="51"/>
     </row>
-    <row r="22" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>19</v>
       </c>
@@ -3126,41 +3705,72 @@
       <c r="O22">
         <v>16</v>
       </c>
-      <c r="AC22" s="37">
+      <c r="AC22" s="45">
         <v>18</v>
       </c>
-      <c r="AD22" s="38"/>
-      <c r="AE22" s="39">
+      <c r="AD22" s="41"/>
+      <c r="AE22" s="40">
         <v>1</v>
       </c>
-      <c r="AF22" s="39"/>
-      <c r="AG22" s="39">
+      <c r="AF22" s="40"/>
+      <c r="AG22" s="40">
         <v>3</v>
       </c>
-      <c r="AH22" s="39"/>
-      <c r="AI22" s="39">
+      <c r="AH22" s="40"/>
+      <c r="AI22" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ22" s="38"/>
-      <c r="AO22" s="37">
+      <c r="AJ22" s="41"/>
+      <c r="AO22" s="45">
         <v>18</v>
       </c>
-      <c r="AP22" s="38"/>
-      <c r="AQ22" s="37">
+      <c r="AP22" s="41"/>
+      <c r="AQ22" s="45">
         <v>21</v>
       </c>
-      <c r="AR22" s="39"/>
-      <c r="AS22" s="39">
+      <c r="AR22" s="40"/>
+      <c r="AS22" s="40">
         <v>23</v>
       </c>
-      <c r="AT22" s="39"/>
-      <c r="AU22" s="39">
+      <c r="AT22" s="40"/>
+      <c r="AU22" s="40">
         <v>22</v>
       </c>
-      <c r="AV22" s="38"/>
-      <c r="AW22" s="50"/>
+      <c r="AV22" s="41"/>
+      <c r="AW22" s="51"/>
+      <c r="BB22" s="45">
+        <v>17</v>
+      </c>
+      <c r="BC22" s="41"/>
+      <c r="BD22" s="45">
+        <v>690</v>
+      </c>
+      <c r="BE22" s="40"/>
+      <c r="BF22" s="40"/>
+      <c r="BG22" s="40">
+        <v>580</v>
+      </c>
+      <c r="BH22" s="40"/>
+      <c r="BI22" s="41"/>
+      <c r="BN22" s="45">
+        <v>18</v>
+      </c>
+      <c r="BO22" s="41"/>
+      <c r="BP22" s="45">
+        <v>21</v>
+      </c>
+      <c r="BQ22" s="40"/>
+      <c r="BR22" s="40">
+        <v>23</v>
+      </c>
+      <c r="BS22" s="40"/>
+      <c r="BT22" s="40">
+        <v>22</v>
+      </c>
+      <c r="BU22" s="41"/>
+      <c r="BV22" s="51"/>
     </row>
-    <row r="23" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H23" s="10"/>
       <c r="I23" s="15"/>
       <c r="J23" s="13"/>
@@ -3168,85 +3778,149 @@
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
-      <c r="AC23" s="37">
+      <c r="AC23" s="45">
         <v>19</v>
       </c>
-      <c r="AD23" s="38"/>
-      <c r="AE23" s="39">
+      <c r="AD23" s="41"/>
+      <c r="AE23" s="40">
         <v>5</v>
       </c>
-      <c r="AF23" s="39"/>
-      <c r="AG23" s="39">
+      <c r="AF23" s="40"/>
+      <c r="AG23" s="40">
         <v>3</v>
       </c>
-      <c r="AH23" s="39"/>
-      <c r="AI23" s="39">
+      <c r="AH23" s="40"/>
+      <c r="AI23" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ23" s="38"/>
-      <c r="AO23" s="37">
+      <c r="AJ23" s="41"/>
+      <c r="AO23" s="45">
         <v>19</v>
       </c>
-      <c r="AP23" s="38"/>
-      <c r="AQ23" s="39">
+      <c r="AP23" s="41"/>
+      <c r="AQ23" s="40">
         <v>21</v>
       </c>
-      <c r="AR23" s="39"/>
-      <c r="AS23" s="39">
+      <c r="AR23" s="40"/>
+      <c r="AS23" s="40">
         <v>22</v>
       </c>
-      <c r="AT23" s="39"/>
-      <c r="AU23" s="39">
+      <c r="AT23" s="40"/>
+      <c r="AU23" s="40">
         <v>20</v>
       </c>
-      <c r="AV23" s="38"/>
-      <c r="AW23" s="51"/>
+      <c r="AV23" s="41"/>
+      <c r="AW23" s="52"/>
+      <c r="BB23" s="45">
+        <v>18</v>
+      </c>
+      <c r="BC23" s="41"/>
+      <c r="BD23" s="45">
+        <v>610</v>
+      </c>
+      <c r="BE23" s="40"/>
+      <c r="BF23" s="40"/>
+      <c r="BG23" s="40">
+        <v>580</v>
+      </c>
+      <c r="BH23" s="40"/>
+      <c r="BI23" s="41"/>
+      <c r="BN23" s="45">
+        <v>19</v>
+      </c>
+      <c r="BO23" s="41"/>
+      <c r="BP23" s="40">
+        <v>21</v>
+      </c>
+      <c r="BQ23" s="40"/>
+      <c r="BR23" s="40">
+        <v>22</v>
+      </c>
+      <c r="BS23" s="40"/>
+      <c r="BT23" s="40">
+        <v>20</v>
+      </c>
+      <c r="BU23" s="41"/>
+      <c r="BV23" s="52"/>
     </row>
-    <row r="24" spans="3:49" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I24" s="16"/>
       <c r="J24" s="6"/>
-      <c r="AC24" s="37">
+      <c r="AC24" s="45">
         <v>20</v>
       </c>
-      <c r="AD24" s="38"/>
-      <c r="AE24" s="39">
+      <c r="AD24" s="41"/>
+      <c r="AE24" s="40">
         <v>-5</v>
       </c>
-      <c r="AF24" s="39"/>
-      <c r="AG24" s="39">
+      <c r="AF24" s="40"/>
+      <c r="AG24" s="40">
         <v>-1</v>
       </c>
-      <c r="AH24" s="39"/>
-      <c r="AI24" s="39">
+      <c r="AH24" s="40"/>
+      <c r="AI24" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ24" s="38"/>
-      <c r="AO24" s="37">
+      <c r="AJ24" s="41"/>
+      <c r="AO24" s="45">
         <v>20</v>
       </c>
-      <c r="AP24" s="38"/>
-      <c r="AQ24" s="52">
+      <c r="AP24" s="41"/>
+      <c r="AQ24" s="49">
         <v>0</v>
       </c>
-      <c r="AR24" s="52"/>
-      <c r="AS24" s="52">
+      <c r="AR24" s="49"/>
+      <c r="AS24" s="49">
         <v>14</v>
       </c>
-      <c r="AT24" s="52"/>
-      <c r="AU24" s="52">
+      <c r="AT24" s="49"/>
+      <c r="AU24" s="49">
         <v>16</v>
       </c>
-      <c r="AV24" s="52"/>
+      <c r="AV24" s="49"/>
       <c r="AW24" s="46" t="s">
         <v>7</v>
       </c>
+      <c r="BB24" s="45">
+        <v>19</v>
+      </c>
+      <c r="BC24" s="41"/>
+      <c r="BD24" s="45">
+        <v>450</v>
+      </c>
+      <c r="BE24" s="40"/>
+      <c r="BF24" s="40"/>
+      <c r="BG24" s="40">
+        <v>580</v>
+      </c>
+      <c r="BH24" s="40"/>
+      <c r="BI24" s="41"/>
+      <c r="BN24" s="45">
+        <v>20</v>
+      </c>
+      <c r="BO24" s="41"/>
+      <c r="BP24" s="49">
+        <v>0</v>
+      </c>
+      <c r="BQ24" s="49"/>
+      <c r="BR24" s="49">
+        <v>14</v>
+      </c>
+      <c r="BS24" s="49"/>
+      <c r="BT24" s="49">
+        <v>16</v>
+      </c>
+      <c r="BU24" s="49"/>
+      <c r="BV24" s="46" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="25" spans="3:49" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="43" t="s">
+    <row r="25" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
       <c r="I25" s="16"/>
       <c r="J25" s="6"/>
       <c r="L25">
@@ -3255,41 +3929,72 @@
       <c r="O25">
         <v>20</v>
       </c>
-      <c r="AC25" s="37">
+      <c r="AC25" s="45">
         <v>21</v>
       </c>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="39">
+      <c r="AD25" s="41"/>
+      <c r="AE25" s="40">
         <v>-3</v>
       </c>
-      <c r="AF25" s="39"/>
-      <c r="AG25" s="39">
+      <c r="AF25" s="40"/>
+      <c r="AG25" s="40">
         <v>-1</v>
       </c>
-      <c r="AH25" s="39"/>
-      <c r="AI25" s="39">
+      <c r="AH25" s="40"/>
+      <c r="AI25" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ25" s="38"/>
-      <c r="AO25" s="37">
+      <c r="AJ25" s="41"/>
+      <c r="AO25" s="45">
         <v>21</v>
       </c>
-      <c r="AP25" s="38"/>
-      <c r="AQ25" s="52">
+      <c r="AP25" s="41"/>
+      <c r="AQ25" s="49">
         <v>0</v>
       </c>
-      <c r="AR25" s="52"/>
-      <c r="AS25" s="52">
+      <c r="AR25" s="49"/>
+      <c r="AS25" s="49">
         <v>16</v>
       </c>
-      <c r="AT25" s="52"/>
-      <c r="AU25" s="52">
+      <c r="AT25" s="49"/>
+      <c r="AU25" s="49">
         <v>2</v>
       </c>
-      <c r="AV25" s="52"/>
+      <c r="AV25" s="49"/>
       <c r="AW25" s="47"/>
+      <c r="BB25" s="45">
+        <v>20</v>
+      </c>
+      <c r="BC25" s="41"/>
+      <c r="BD25" s="45">
+        <v>850</v>
+      </c>
+      <c r="BE25" s="40"/>
+      <c r="BF25" s="40"/>
+      <c r="BG25" s="40">
+        <v>740</v>
+      </c>
+      <c r="BH25" s="40"/>
+      <c r="BI25" s="41"/>
+      <c r="BN25" s="45">
+        <v>21</v>
+      </c>
+      <c r="BO25" s="41"/>
+      <c r="BP25" s="49">
+        <v>0</v>
+      </c>
+      <c r="BQ25" s="49"/>
+      <c r="BR25" s="49">
+        <v>16</v>
+      </c>
+      <c r="BS25" s="49"/>
+      <c r="BT25" s="49">
+        <v>2</v>
+      </c>
+      <c r="BU25" s="49"/>
+      <c r="BV25" s="47"/>
     </row>
-    <row r="26" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
@@ -3300,41 +4005,72 @@
       <c r="J26" s="6"/>
       <c r="M26" s="3"/>
       <c r="N26" s="2"/>
-      <c r="AC26" s="37">
+      <c r="AC26" s="45">
         <v>22</v>
       </c>
-      <c r="AD26" s="38"/>
-      <c r="AE26" s="39">
+      <c r="AD26" s="41"/>
+      <c r="AE26" s="40">
         <v>-5</v>
       </c>
-      <c r="AF26" s="39"/>
-      <c r="AG26" s="39">
+      <c r="AF26" s="40"/>
+      <c r="AG26" s="40">
         <v>-3</v>
       </c>
-      <c r="AH26" s="39"/>
-      <c r="AI26" s="39">
+      <c r="AH26" s="40"/>
+      <c r="AI26" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ26" s="38"/>
-      <c r="AO26" s="37">
+      <c r="AJ26" s="41"/>
+      <c r="AO26" s="45">
         <v>22</v>
       </c>
-      <c r="AP26" s="38"/>
-      <c r="AQ26" s="52">
+      <c r="AP26" s="41"/>
+      <c r="AQ26" s="49">
         <v>3</v>
       </c>
-      <c r="AR26" s="52"/>
-      <c r="AS26" s="52">
+      <c r="AR26" s="49"/>
+      <c r="AS26" s="49">
         <v>17</v>
       </c>
-      <c r="AT26" s="52"/>
-      <c r="AU26" s="52">
+      <c r="AT26" s="49"/>
+      <c r="AU26" s="49">
         <v>24</v>
       </c>
-      <c r="AV26" s="52"/>
+      <c r="AV26" s="49"/>
       <c r="AW26" s="47"/>
+      <c r="BB26" s="45">
+        <v>21</v>
+      </c>
+      <c r="BC26" s="41"/>
+      <c r="BD26" s="45">
+        <v>770</v>
+      </c>
+      <c r="BE26" s="40"/>
+      <c r="BF26" s="40"/>
+      <c r="BG26" s="40">
+        <v>740</v>
+      </c>
+      <c r="BH26" s="40"/>
+      <c r="BI26" s="41"/>
+      <c r="BN26" s="45">
+        <v>22</v>
+      </c>
+      <c r="BO26" s="41"/>
+      <c r="BP26" s="49">
+        <v>3</v>
+      </c>
+      <c r="BQ26" s="49"/>
+      <c r="BR26" s="49">
+        <v>17</v>
+      </c>
+      <c r="BS26" s="49"/>
+      <c r="BT26" s="49">
+        <v>24</v>
+      </c>
+      <c r="BU26" s="49"/>
+      <c r="BV26" s="47"/>
     </row>
-    <row r="27" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
@@ -3356,41 +4092,72 @@
       <c r="O27">
         <v>22</v>
       </c>
-      <c r="AC27" s="37">
+      <c r="AC27" s="45">
         <v>23</v>
       </c>
-      <c r="AD27" s="38"/>
-      <c r="AE27" s="39">
+      <c r="AD27" s="41"/>
+      <c r="AE27" s="40">
         <v>-3</v>
       </c>
-      <c r="AF27" s="39"/>
-      <c r="AG27" s="39">
+      <c r="AF27" s="40"/>
+      <c r="AG27" s="40">
         <v>-3</v>
       </c>
-      <c r="AH27" s="39"/>
-      <c r="AI27" s="39">
+      <c r="AH27" s="40"/>
+      <c r="AI27" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ27" s="38"/>
-      <c r="AO27" s="37">
+      <c r="AJ27" s="41"/>
+      <c r="AO27" s="45">
         <v>23</v>
       </c>
-      <c r="AP27" s="38"/>
-      <c r="AQ27" s="52">
+      <c r="AP27" s="41"/>
+      <c r="AQ27" s="49">
         <v>3</v>
       </c>
-      <c r="AR27" s="52"/>
-      <c r="AS27" s="52">
+      <c r="AR27" s="49"/>
+      <c r="AS27" s="49">
         <v>24</v>
       </c>
-      <c r="AT27" s="52"/>
-      <c r="AU27" s="52">
+      <c r="AT27" s="49"/>
+      <c r="AU27" s="49">
         <v>10</v>
       </c>
-      <c r="AV27" s="52"/>
+      <c r="AV27" s="49"/>
       <c r="AW27" s="47"/>
+      <c r="BB27" s="45">
+        <v>22</v>
+      </c>
+      <c r="BC27" s="41"/>
+      <c r="BD27" s="45">
+        <v>850</v>
+      </c>
+      <c r="BE27" s="40"/>
+      <c r="BF27" s="40"/>
+      <c r="BG27" s="40">
+        <v>820</v>
+      </c>
+      <c r="BH27" s="40"/>
+      <c r="BI27" s="41"/>
+      <c r="BN27" s="45">
+        <v>23</v>
+      </c>
+      <c r="BO27" s="41"/>
+      <c r="BP27" s="49">
+        <v>3</v>
+      </c>
+      <c r="BQ27" s="49"/>
+      <c r="BR27" s="49">
+        <v>24</v>
+      </c>
+      <c r="BS27" s="49"/>
+      <c r="BT27" s="49">
+        <v>10</v>
+      </c>
+      <c r="BU27" s="49"/>
+      <c r="BV27" s="47"/>
     </row>
-    <row r="28" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
@@ -3403,41 +4170,72 @@
       <c r="L28" s="1"/>
       <c r="M28" s="30"/>
       <c r="N28" s="22"/>
-      <c r="AC28" s="37">
+      <c r="AC28" s="45">
         <v>24</v>
       </c>
-      <c r="AD28" s="38"/>
-      <c r="AE28" s="39">
+      <c r="AD28" s="41"/>
+      <c r="AE28" s="40">
         <v>-1</v>
       </c>
-      <c r="AF28" s="39"/>
-      <c r="AG28" s="39">
+      <c r="AF28" s="40"/>
+      <c r="AG28" s="40">
         <v>-3</v>
       </c>
-      <c r="AH28" s="39"/>
-      <c r="AI28" s="39">
+      <c r="AH28" s="40"/>
+      <c r="AI28" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ28" s="38"/>
-      <c r="AO28" s="37">
+      <c r="AJ28" s="41"/>
+      <c r="AO28" s="45">
         <v>24</v>
       </c>
-      <c r="AP28" s="38"/>
-      <c r="AQ28" s="52">
+      <c r="AP28" s="41"/>
+      <c r="AQ28" s="49">
         <v>6</v>
       </c>
-      <c r="AR28" s="52"/>
-      <c r="AS28" s="52">
+      <c r="AR28" s="49"/>
+      <c r="AS28" s="49">
         <v>20</v>
       </c>
-      <c r="AT28" s="52"/>
-      <c r="AU28" s="52">
+      <c r="AT28" s="49"/>
+      <c r="AU28" s="49">
         <v>22</v>
       </c>
-      <c r="AV28" s="52"/>
+      <c r="AV28" s="49"/>
       <c r="AW28" s="47"/>
+      <c r="BB28" s="45">
+        <v>23</v>
+      </c>
+      <c r="BC28" s="41"/>
+      <c r="BD28" s="45">
+        <v>770</v>
+      </c>
+      <c r="BE28" s="40"/>
+      <c r="BF28" s="40"/>
+      <c r="BG28" s="40">
+        <v>820</v>
+      </c>
+      <c r="BH28" s="40"/>
+      <c r="BI28" s="41"/>
+      <c r="BN28" s="45">
+        <v>24</v>
+      </c>
+      <c r="BO28" s="41"/>
+      <c r="BP28" s="49">
+        <v>6</v>
+      </c>
+      <c r="BQ28" s="49"/>
+      <c r="BR28" s="49">
+        <v>20</v>
+      </c>
+      <c r="BS28" s="49"/>
+      <c r="BT28" s="49">
+        <v>22</v>
+      </c>
+      <c r="BU28" s="49"/>
+      <c r="BV28" s="47"/>
     </row>
-    <row r="29" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
@@ -3449,41 +4247,72 @@
       <c r="K29" s="32"/>
       <c r="L29" s="27"/>
       <c r="M29" s="31"/>
-      <c r="AC29" s="37">
+      <c r="AC29" s="45">
         <v>25</v>
       </c>
-      <c r="AD29" s="38"/>
-      <c r="AE29" s="39">
+      <c r="AD29" s="41"/>
+      <c r="AE29" s="40">
         <v>1</v>
       </c>
-      <c r="AF29" s="39"/>
-      <c r="AG29" s="39">
+      <c r="AF29" s="40"/>
+      <c r="AG29" s="40">
         <v>-3</v>
       </c>
-      <c r="AH29" s="39"/>
-      <c r="AI29" s="39">
+      <c r="AH29" s="40"/>
+      <c r="AI29" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ29" s="38"/>
-      <c r="AO29" s="37">
+      <c r="AJ29" s="41"/>
+      <c r="AO29" s="45">
         <v>25</v>
       </c>
-      <c r="AP29" s="38"/>
-      <c r="AQ29" s="52">
+      <c r="AP29" s="41"/>
+      <c r="AQ29" s="49">
         <v>6</v>
       </c>
-      <c r="AR29" s="52"/>
-      <c r="AS29" s="52">
+      <c r="AR29" s="49"/>
+      <c r="AS29" s="49">
         <v>22</v>
       </c>
-      <c r="AT29" s="52"/>
-      <c r="AU29" s="52">
+      <c r="AT29" s="49"/>
+      <c r="AU29" s="49">
         <v>8</v>
       </c>
-      <c r="AV29" s="52"/>
+      <c r="AV29" s="49"/>
       <c r="AW29" s="47"/>
+      <c r="BB29" s="45">
+        <v>24</v>
+      </c>
+      <c r="BC29" s="41"/>
+      <c r="BD29" s="45">
+        <v>690</v>
+      </c>
+      <c r="BE29" s="40"/>
+      <c r="BF29" s="40"/>
+      <c r="BG29" s="40">
+        <v>820</v>
+      </c>
+      <c r="BH29" s="40"/>
+      <c r="BI29" s="41"/>
+      <c r="BN29" s="45">
+        <v>25</v>
+      </c>
+      <c r="BO29" s="41"/>
+      <c r="BP29" s="49">
+        <v>6</v>
+      </c>
+      <c r="BQ29" s="49"/>
+      <c r="BR29" s="49">
+        <v>22</v>
+      </c>
+      <c r="BS29" s="49"/>
+      <c r="BT29" s="49">
+        <v>8</v>
+      </c>
+      <c r="BU29" s="49"/>
+      <c r="BV29" s="47"/>
     </row>
-    <row r="30" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
@@ -3499,41 +4328,72 @@
       <c r="M30">
         <v>26</v>
       </c>
-      <c r="AC30" s="37">
+      <c r="AC30" s="45">
         <v>26</v>
       </c>
-      <c r="AD30" s="38"/>
-      <c r="AE30" s="39">
+      <c r="AD30" s="41"/>
+      <c r="AE30" s="40">
         <v>-3</v>
       </c>
-      <c r="AF30" s="39"/>
-      <c r="AG30" s="39">
+      <c r="AF30" s="40"/>
+      <c r="AG30" s="40">
         <v>-5</v>
       </c>
-      <c r="AH30" s="39"/>
-      <c r="AI30" s="39">
+      <c r="AH30" s="40"/>
+      <c r="AI30" s="40">
         <v>-1</v>
       </c>
-      <c r="AJ30" s="38"/>
-      <c r="AO30" s="37">
+      <c r="AJ30" s="41"/>
+      <c r="AO30" s="45">
         <v>26</v>
       </c>
-      <c r="AP30" s="38"/>
-      <c r="AQ30" s="52">
+      <c r="AP30" s="41"/>
+      <c r="AQ30" s="49">
         <v>22</v>
       </c>
-      <c r="AR30" s="52"/>
-      <c r="AS30" s="52">
+      <c r="AR30" s="49"/>
+      <c r="AS30" s="49">
         <v>26</v>
       </c>
-      <c r="AT30" s="52"/>
-      <c r="AU30" s="52">
+      <c r="AT30" s="49"/>
+      <c r="AU30" s="49">
         <v>12</v>
       </c>
-      <c r="AV30" s="52"/>
+      <c r="AV30" s="49"/>
       <c r="AW30" s="47"/>
+      <c r="BB30" s="45">
+        <v>25</v>
+      </c>
+      <c r="BC30" s="41"/>
+      <c r="BD30" s="45">
+        <v>610</v>
+      </c>
+      <c r="BE30" s="40"/>
+      <c r="BF30" s="40"/>
+      <c r="BG30" s="40">
+        <v>820</v>
+      </c>
+      <c r="BH30" s="40"/>
+      <c r="BI30" s="41"/>
+      <c r="BN30" s="45">
+        <v>26</v>
+      </c>
+      <c r="BO30" s="41"/>
+      <c r="BP30" s="49">
+        <v>22</v>
+      </c>
+      <c r="BQ30" s="49"/>
+      <c r="BR30" s="49">
+        <v>26</v>
+      </c>
+      <c r="BS30" s="49"/>
+      <c r="BT30" s="49">
+        <v>12</v>
+      </c>
+      <c r="BU30" s="49"/>
+      <c r="BV30" s="47"/>
     </row>
-    <row r="31" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D31">
         <v>14</v>
       </c>
@@ -3549,66 +4409,130 @@
       <c r="Q31">
         <v>18</v>
       </c>
-      <c r="AC31" s="53">
+      <c r="AC31" s="44">
         <v>27</v>
       </c>
-      <c r="AD31" s="54"/>
-      <c r="AE31" s="53">
+      <c r="AD31" s="43"/>
+      <c r="AE31" s="44">
         <v>-1</v>
       </c>
-      <c r="AF31" s="55"/>
-      <c r="AG31" s="55">
+      <c r="AF31" s="42"/>
+      <c r="AG31" s="42">
         <v>-5</v>
       </c>
-      <c r="AH31" s="55"/>
-      <c r="AI31" s="55">
+      <c r="AH31" s="42"/>
+      <c r="AI31" s="42">
         <v>-1</v>
       </c>
-      <c r="AJ31" s="54"/>
-      <c r="AO31" s="37">
+      <c r="AJ31" s="43"/>
+      <c r="AO31" s="45">
         <v>27</v>
       </c>
-      <c r="AP31" s="38"/>
-      <c r="AQ31" s="52">
+      <c r="AP31" s="41"/>
+      <c r="AQ31" s="49">
         <v>22</v>
       </c>
-      <c r="AR31" s="52"/>
-      <c r="AS31" s="52">
+      <c r="AR31" s="49"/>
+      <c r="AS31" s="49">
         <v>12</v>
       </c>
-      <c r="AT31" s="52"/>
-      <c r="AU31" s="52">
+      <c r="AT31" s="49"/>
+      <c r="AU31" s="49">
         <v>8</v>
       </c>
-      <c r="AV31" s="52"/>
+      <c r="AV31" s="49"/>
       <c r="AW31" s="47"/>
+      <c r="BB31" s="45">
+        <v>26</v>
+      </c>
+      <c r="BC31" s="41"/>
+      <c r="BD31" s="45">
+        <v>770</v>
+      </c>
+      <c r="BE31" s="40"/>
+      <c r="BF31" s="40"/>
+      <c r="BG31" s="40">
+        <v>900</v>
+      </c>
+      <c r="BH31" s="40"/>
+      <c r="BI31" s="41"/>
+      <c r="BN31" s="45">
+        <v>27</v>
+      </c>
+      <c r="BO31" s="41"/>
+      <c r="BP31" s="49">
+        <v>22</v>
+      </c>
+      <c r="BQ31" s="49"/>
+      <c r="BR31" s="49">
+        <v>12</v>
+      </c>
+      <c r="BS31" s="49"/>
+      <c r="BT31" s="49">
+        <v>8</v>
+      </c>
+      <c r="BU31" s="49"/>
+      <c r="BV31" s="47"/>
     </row>
-    <row r="32" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E32" s="3"/>
       <c r="F32" s="2"/>
       <c r="N32" s="3"/>
       <c r="O32" s="2"/>
-      <c r="AO32" s="37">
+      <c r="AO32" s="45">
         <v>28</v>
       </c>
-      <c r="AP32" s="38"/>
-      <c r="AQ32" s="52">
+      <c r="AP32" s="41"/>
+      <c r="AQ32" s="49">
         <v>15</v>
       </c>
-      <c r="AR32" s="52"/>
-      <c r="AS32" s="52">
+      <c r="AR32" s="49"/>
+      <c r="AS32" s="49">
         <v>1</v>
       </c>
-      <c r="AT32" s="52"/>
-      <c r="AU32" s="52">
+      <c r="AT32" s="49"/>
+      <c r="AU32" s="49">
         <v>5</v>
       </c>
-      <c r="AV32" s="52"/>
+      <c r="AV32" s="49"/>
       <c r="AW32" s="46" t="s">
         <v>6</v>
       </c>
+      <c r="BB32" s="44">
+        <v>27</v>
+      </c>
+      <c r="BC32" s="43"/>
+      <c r="BD32" s="44">
+        <v>690</v>
+      </c>
+      <c r="BE32" s="42"/>
+      <c r="BF32" s="42"/>
+      <c r="BG32" s="42">
+        <v>900</v>
+      </c>
+      <c r="BH32" s="42"/>
+      <c r="BI32" s="43"/>
+      <c r="BN32" s="45">
+        <v>28</v>
+      </c>
+      <c r="BO32" s="41"/>
+      <c r="BP32" s="49">
+        <v>15</v>
+      </c>
+      <c r="BQ32" s="49"/>
+      <c r="BR32" s="49">
+        <v>1</v>
+      </c>
+      <c r="BS32" s="49"/>
+      <c r="BT32" s="49">
+        <v>5</v>
+      </c>
+      <c r="BU32" s="49"/>
+      <c r="BV32" s="46" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="33" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33">
         <v>17</v>
       </c>
@@ -3634,94 +4558,162 @@
       <c r="P33">
         <v>19</v>
       </c>
-      <c r="AO33" s="37">
+      <c r="AO33" s="45">
         <v>29</v>
       </c>
-      <c r="AP33" s="38"/>
-      <c r="AQ33" s="52">
+      <c r="AP33" s="41"/>
+      <c r="AQ33" s="49">
         <v>15</v>
       </c>
-      <c r="AR33" s="52"/>
-      <c r="AS33" s="52">
+      <c r="AR33" s="49"/>
+      <c r="AS33" s="49">
         <v>5</v>
       </c>
-      <c r="AT33" s="52"/>
-      <c r="AU33" s="52">
+      <c r="AT33" s="49"/>
+      <c r="AU33" s="49">
         <v>19</v>
       </c>
-      <c r="AV33" s="52"/>
+      <c r="AV33" s="49"/>
       <c r="AW33" s="47"/>
+      <c r="BN33" s="45">
+        <v>29</v>
+      </c>
+      <c r="BO33" s="41"/>
+      <c r="BP33" s="49">
+        <v>15</v>
+      </c>
+      <c r="BQ33" s="49"/>
+      <c r="BR33" s="49">
+        <v>5</v>
+      </c>
+      <c r="BS33" s="49"/>
+      <c r="BT33" s="49">
+        <v>19</v>
+      </c>
+      <c r="BU33" s="49"/>
+      <c r="BV33" s="47"/>
     </row>
-    <row r="34" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E34" s="16"/>
       <c r="F34" s="6"/>
       <c r="N34" s="16"/>
       <c r="O34" s="6"/>
-      <c r="AO34" s="37">
+      <c r="AO34" s="45">
         <v>30</v>
       </c>
-      <c r="AP34" s="38"/>
-      <c r="AQ34" s="52">
+      <c r="AP34" s="41"/>
+      <c r="AQ34" s="49">
         <v>18</v>
       </c>
-      <c r="AR34" s="52"/>
-      <c r="AS34" s="52">
+      <c r="AR34" s="49"/>
+      <c r="AS34" s="49">
         <v>4</v>
       </c>
-      <c r="AT34" s="52"/>
-      <c r="AU34" s="52">
+      <c r="AT34" s="49"/>
+      <c r="AU34" s="49">
         <v>11</v>
       </c>
-      <c r="AV34" s="52"/>
+      <c r="AV34" s="49"/>
       <c r="AW34" s="47"/>
+      <c r="BN34" s="45">
+        <v>30</v>
+      </c>
+      <c r="BO34" s="41"/>
+      <c r="BP34" s="49">
+        <v>18</v>
+      </c>
+      <c r="BQ34" s="49"/>
+      <c r="BR34" s="49">
+        <v>4</v>
+      </c>
+      <c r="BS34" s="49"/>
+      <c r="BT34" s="49">
+        <v>11</v>
+      </c>
+      <c r="BU34" s="49"/>
+      <c r="BV34" s="47"/>
     </row>
-    <row r="35" spans="3:49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:74" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E35" s="16"/>
       <c r="F35" s="6"/>
       <c r="N35" s="16"/>
       <c r="O35" s="6"/>
-      <c r="AO35" s="37">
+      <c r="AO35" s="45">
         <v>31</v>
       </c>
-      <c r="AP35" s="38"/>
-      <c r="AQ35" s="52">
+      <c r="AP35" s="41"/>
+      <c r="AQ35" s="49">
         <v>18</v>
       </c>
-      <c r="AR35" s="52"/>
-      <c r="AS35" s="52">
+      <c r="AR35" s="49"/>
+      <c r="AS35" s="49">
         <v>11</v>
       </c>
-      <c r="AT35" s="52"/>
-      <c r="AU35" s="52">
+      <c r="AT35" s="49"/>
+      <c r="AU35" s="49">
         <v>25</v>
       </c>
-      <c r="AV35" s="52"/>
+      <c r="AV35" s="49"/>
       <c r="AW35" s="47"/>
+      <c r="BN35" s="45">
+        <v>31</v>
+      </c>
+      <c r="BO35" s="41"/>
+      <c r="BP35" s="49">
+        <v>18</v>
+      </c>
+      <c r="BQ35" s="49"/>
+      <c r="BR35" s="49">
+        <v>11</v>
+      </c>
+      <c r="BS35" s="49"/>
+      <c r="BT35" s="49">
+        <v>25</v>
+      </c>
+      <c r="BU35" s="49"/>
+      <c r="BV35" s="47"/>
     </row>
-    <row r="36" spans="3:49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:74" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E36" s="16"/>
       <c r="F36" s="6"/>
       <c r="N36" s="16"/>
       <c r="O36" s="6"/>
-      <c r="AO36" s="37">
+      <c r="AO36" s="45">
         <v>32</v>
       </c>
-      <c r="AP36" s="38"/>
-      <c r="AQ36" s="52">
+      <c r="AP36" s="41"/>
+      <c r="AQ36" s="49">
         <v>21</v>
       </c>
-      <c r="AR36" s="52"/>
-      <c r="AS36" s="52">
+      <c r="AR36" s="49"/>
+      <c r="AS36" s="49">
         <v>7</v>
       </c>
-      <c r="AT36" s="52"/>
-      <c r="AU36" s="52">
+      <c r="AT36" s="49"/>
+      <c r="AU36" s="49">
         <v>9</v>
       </c>
-      <c r="AV36" s="52"/>
+      <c r="AV36" s="49"/>
       <c r="AW36" s="47"/>
+      <c r="BN36" s="45">
+        <v>32</v>
+      </c>
+      <c r="BO36" s="41"/>
+      <c r="BP36" s="49">
+        <v>21</v>
+      </c>
+      <c r="BQ36" s="49"/>
+      <c r="BR36" s="49">
+        <v>7</v>
+      </c>
+      <c r="BS36" s="49"/>
+      <c r="BT36" s="49">
+        <v>9</v>
+      </c>
+      <c r="BU36" s="49"/>
+      <c r="BV36" s="47"/>
     </row>
-    <row r="37" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D37">
         <v>20</v>
       </c>
@@ -3741,48 +4733,82 @@
       <c r="Q37">
         <v>23</v>
       </c>
-      <c r="AO37" s="37">
+      <c r="AO37" s="45">
         <v>33</v>
       </c>
-      <c r="AP37" s="38"/>
-      <c r="AQ37" s="52">
+      <c r="AP37" s="41"/>
+      <c r="AQ37" s="49">
         <v>21</v>
       </c>
-      <c r="AR37" s="52"/>
-      <c r="AS37" s="52">
+      <c r="AR37" s="49"/>
+      <c r="AS37" s="49">
         <v>9</v>
       </c>
-      <c r="AT37" s="52"/>
-      <c r="AU37" s="52">
+      <c r="AT37" s="49"/>
+      <c r="AU37" s="49">
         <v>23</v>
       </c>
-      <c r="AV37" s="52"/>
+      <c r="AV37" s="49"/>
       <c r="AW37" s="47"/>
+      <c r="BN37" s="45">
+        <v>33</v>
+      </c>
+      <c r="BO37" s="41"/>
+      <c r="BP37" s="49">
+        <v>21</v>
+      </c>
+      <c r="BQ37" s="49"/>
+      <c r="BR37" s="49">
+        <v>9</v>
+      </c>
+      <c r="BS37" s="49"/>
+      <c r="BT37" s="49">
+        <v>23</v>
+      </c>
+      <c r="BU37" s="49"/>
+      <c r="BV37" s="47"/>
     </row>
-    <row r="38" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E38" s="3"/>
       <c r="F38" s="2"/>
       <c r="N38" s="3"/>
       <c r="O38" s="2"/>
-      <c r="AO38" s="37">
+      <c r="AO38" s="45">
         <v>34</v>
       </c>
-      <c r="AP38" s="38"/>
-      <c r="AQ38" s="52">
+      <c r="AP38" s="41"/>
+      <c r="AQ38" s="49">
         <v>11</v>
       </c>
-      <c r="AR38" s="52"/>
-      <c r="AS38" s="52">
+      <c r="AR38" s="49"/>
+      <c r="AS38" s="49">
         <v>13</v>
       </c>
-      <c r="AT38" s="52"/>
-      <c r="AU38" s="52">
+      <c r="AT38" s="49"/>
+      <c r="AU38" s="49">
         <v>27</v>
       </c>
-      <c r="AV38" s="52"/>
+      <c r="AV38" s="49"/>
       <c r="AW38" s="47"/>
+      <c r="BN38" s="45">
+        <v>34</v>
+      </c>
+      <c r="BO38" s="41"/>
+      <c r="BP38" s="49">
+        <v>11</v>
+      </c>
+      <c r="BQ38" s="49"/>
+      <c r="BR38" s="49">
+        <v>13</v>
+      </c>
+      <c r="BS38" s="49"/>
+      <c r="BT38" s="49">
+        <v>27</v>
+      </c>
+      <c r="BU38" s="49"/>
+      <c r="BV38" s="47"/>
     </row>
-    <row r="39" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39">
         <v>24</v>
       </c>
@@ -3808,50 +4834,86 @@
       <c r="P39">
         <v>25</v>
       </c>
-      <c r="AO39" s="37">
+      <c r="AO39" s="45">
         <v>35</v>
       </c>
-      <c r="AP39" s="38"/>
-      <c r="AQ39" s="39">
+      <c r="AP39" s="41"/>
+      <c r="AQ39" s="40">
         <v>11</v>
       </c>
-      <c r="AR39" s="39"/>
-      <c r="AS39" s="39">
+      <c r="AR39" s="40"/>
+      <c r="AS39" s="40">
         <v>27</v>
       </c>
-      <c r="AT39" s="39"/>
-      <c r="AU39" s="39">
+      <c r="AT39" s="40"/>
+      <c r="AU39" s="40">
         <v>25</v>
       </c>
-      <c r="AV39" s="39"/>
+      <c r="AV39" s="40"/>
       <c r="AW39" s="48"/>
+      <c r="BN39" s="45">
+        <v>35</v>
+      </c>
+      <c r="BO39" s="41"/>
+      <c r="BP39" s="40">
+        <v>11</v>
+      </c>
+      <c r="BQ39" s="40"/>
+      <c r="BR39" s="40">
+        <v>27</v>
+      </c>
+      <c r="BS39" s="40"/>
+      <c r="BT39" s="40">
+        <v>25</v>
+      </c>
+      <c r="BU39" s="40"/>
+      <c r="BV39" s="48"/>
     </row>
-    <row r="40" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E40" s="16"/>
       <c r="F40" s="6"/>
       <c r="N40" s="16"/>
       <c r="O40" s="6"/>
-      <c r="AO40" s="37">
+      <c r="AO40" s="45">
         <v>36</v>
       </c>
-      <c r="AP40" s="38"/>
-      <c r="AQ40" s="37">
+      <c r="AP40" s="41"/>
+      <c r="AQ40" s="45">
         <v>15</v>
       </c>
-      <c r="AR40" s="39"/>
-      <c r="AS40" s="39">
+      <c r="AR40" s="40"/>
+      <c r="AS40" s="40">
         <v>14</v>
       </c>
-      <c r="AT40" s="39"/>
-      <c r="AU40" s="39">
+      <c r="AT40" s="40"/>
+      <c r="AU40" s="40">
         <v>0</v>
       </c>
-      <c r="AV40" s="38"/>
+      <c r="AV40" s="41"/>
       <c r="AW40" s="46" t="s">
         <v>9</v>
       </c>
+      <c r="BN40" s="45">
+        <v>36</v>
+      </c>
+      <c r="BO40" s="41"/>
+      <c r="BP40" s="45">
+        <v>15</v>
+      </c>
+      <c r="BQ40" s="40"/>
+      <c r="BR40" s="40">
+        <v>14</v>
+      </c>
+      <c r="BS40" s="40"/>
+      <c r="BT40" s="40">
+        <v>0</v>
+      </c>
+      <c r="BU40" s="41"/>
+      <c r="BV40" s="46" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="41" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D41">
         <v>26</v>
       </c>
@@ -3868,140 +4930,244 @@
       <c r="P41">
         <v>27</v>
       </c>
-      <c r="AO41" s="37">
+      <c r="AO41" s="45">
         <v>37</v>
       </c>
-      <c r="AP41" s="38"/>
-      <c r="AQ41" s="37">
+      <c r="AP41" s="41"/>
+      <c r="AQ41" s="45">
         <v>15</v>
       </c>
-      <c r="AR41" s="39"/>
-      <c r="AS41" s="39">
+      <c r="AR41" s="40"/>
+      <c r="AS41" s="40">
         <v>0</v>
       </c>
-      <c r="AT41" s="39"/>
-      <c r="AU41" s="39">
+      <c r="AT41" s="40"/>
+      <c r="AU41" s="40">
         <v>1</v>
       </c>
-      <c r="AV41" s="38"/>
+      <c r="AV41" s="41"/>
       <c r="AW41" s="47"/>
+      <c r="BN41" s="45">
+        <v>37</v>
+      </c>
+      <c r="BO41" s="41"/>
+      <c r="BP41" s="45">
+        <v>15</v>
+      </c>
+      <c r="BQ41" s="40"/>
+      <c r="BR41" s="40">
+        <v>0</v>
+      </c>
+      <c r="BS41" s="40"/>
+      <c r="BT41" s="40">
+        <v>1</v>
+      </c>
+      <c r="BU41" s="41"/>
+      <c r="BV41" s="47"/>
     </row>
-    <row r="42" spans="3:49" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AO42" s="37">
+    <row r="42" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AO42" s="45">
         <v>38</v>
       </c>
-      <c r="AP42" s="38"/>
-      <c r="AQ42" s="37">
+      <c r="AP42" s="41"/>
+      <c r="AQ42" s="45">
         <v>21</v>
       </c>
-      <c r="AR42" s="39"/>
-      <c r="AS42" s="39">
+      <c r="AR42" s="40"/>
+      <c r="AS42" s="40">
         <v>20</v>
       </c>
-      <c r="AT42" s="39"/>
-      <c r="AU42" s="39">
+      <c r="AT42" s="40"/>
+      <c r="AU42" s="40">
         <v>6</v>
       </c>
-      <c r="AV42" s="38"/>
+      <c r="AV42" s="41"/>
       <c r="AW42" s="47"/>
+      <c r="BN42" s="45">
+        <v>38</v>
+      </c>
+      <c r="BO42" s="41"/>
+      <c r="BP42" s="45">
+        <v>21</v>
+      </c>
+      <c r="BQ42" s="40"/>
+      <c r="BR42" s="40">
+        <v>20</v>
+      </c>
+      <c r="BS42" s="40"/>
+      <c r="BT42" s="40">
+        <v>6</v>
+      </c>
+      <c r="BU42" s="41"/>
+      <c r="BV42" s="47"/>
     </row>
-    <row r="43" spans="3:49" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="43" t="s">
+    <row r="43" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E43" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="45"/>
-      <c r="N43" s="43" t="s">
+      <c r="F43" s="39"/>
+      <c r="N43" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="O43" s="45"/>
-      <c r="AO43" s="37">
+      <c r="O43" s="39"/>
+      <c r="AO43" s="45">
         <v>39</v>
       </c>
-      <c r="AP43" s="38"/>
-      <c r="AQ43" s="37">
+      <c r="AP43" s="41"/>
+      <c r="AQ43" s="45">
         <v>21</v>
       </c>
-      <c r="AR43" s="39"/>
-      <c r="AS43" s="39">
+      <c r="AR43" s="40"/>
+      <c r="AS43" s="40">
         <v>6</v>
       </c>
-      <c r="AT43" s="39"/>
-      <c r="AU43" s="39">
+      <c r="AT43" s="40"/>
+      <c r="AU43" s="40">
         <v>7</v>
       </c>
-      <c r="AV43" s="38"/>
+      <c r="AV43" s="41"/>
       <c r="AW43" s="47"/>
+      <c r="BN43" s="45">
+        <v>39</v>
+      </c>
+      <c r="BO43" s="41"/>
+      <c r="BP43" s="45">
+        <v>21</v>
+      </c>
+      <c r="BQ43" s="40"/>
+      <c r="BR43" s="40">
+        <v>6</v>
+      </c>
+      <c r="BS43" s="40"/>
+      <c r="BT43" s="40">
+        <v>7</v>
+      </c>
+      <c r="BU43" s="41"/>
+      <c r="BV43" s="47"/>
     </row>
-    <row r="44" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="AO44" s="37">
+    <row r="44" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AO44" s="45">
         <v>40</v>
       </c>
-      <c r="AP44" s="38"/>
-      <c r="AQ44" s="37">
+      <c r="AP44" s="41"/>
+      <c r="AQ44" s="45">
         <v>23</v>
       </c>
-      <c r="AR44" s="39"/>
-      <c r="AS44" s="39">
+      <c r="AR44" s="40"/>
+      <c r="AS44" s="40">
         <v>9</v>
       </c>
-      <c r="AT44" s="39"/>
-      <c r="AU44" s="39">
+      <c r="AT44" s="40"/>
+      <c r="AU44" s="40">
         <v>10</v>
       </c>
-      <c r="AV44" s="38"/>
+      <c r="AV44" s="41"/>
       <c r="AW44" s="47"/>
+      <c r="BN44" s="45">
+        <v>40</v>
+      </c>
+      <c r="BO44" s="41"/>
+      <c r="BP44" s="45">
+        <v>23</v>
+      </c>
+      <c r="BQ44" s="40"/>
+      <c r="BR44" s="40">
+        <v>9</v>
+      </c>
+      <c r="BS44" s="40"/>
+      <c r="BT44" s="40">
+        <v>10</v>
+      </c>
+      <c r="BU44" s="41"/>
+      <c r="BV44" s="47"/>
     </row>
-    <row r="45" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AO45" s="37">
+    <row r="45" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AO45" s="45">
         <v>41</v>
       </c>
-      <c r="AP45" s="38"/>
-      <c r="AQ45" s="37">
+      <c r="AP45" s="41"/>
+      <c r="AQ45" s="45">
         <v>23</v>
       </c>
-      <c r="AR45" s="39"/>
-      <c r="AS45" s="39">
+      <c r="AR45" s="40"/>
+      <c r="AS45" s="40">
         <v>10</v>
       </c>
-      <c r="AT45" s="39"/>
-      <c r="AU45" s="39">
+      <c r="AT45" s="40"/>
+      <c r="AU45" s="40">
         <v>24</v>
       </c>
-      <c r="AV45" s="38"/>
+      <c r="AV45" s="41"/>
       <c r="AW45" s="48"/>
+      <c r="BN45" s="45">
+        <v>41</v>
+      </c>
+      <c r="BO45" s="41"/>
+      <c r="BP45" s="45">
+        <v>23</v>
+      </c>
+      <c r="BQ45" s="40"/>
+      <c r="BR45" s="40">
+        <v>10</v>
+      </c>
+      <c r="BS45" s="40"/>
+      <c r="BT45" s="40">
+        <v>24</v>
+      </c>
+      <c r="BU45" s="41"/>
+      <c r="BV45" s="48"/>
     </row>
-    <row r="46" spans="3:49" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I46" s="43" t="s">
+    <row r="46" spans="3:74" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I46" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="45"/>
-      <c r="W46" s="43" t="s">
+      <c r="J46" s="39"/>
+      <c r="W46" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="X46" s="44"/>
-      <c r="Y46" s="44"/>
-      <c r="Z46" s="45"/>
-      <c r="AO46" s="37">
+      <c r="X46" s="38"/>
+      <c r="Y46" s="38"/>
+      <c r="Z46" s="39"/>
+      <c r="AO46" s="45">
         <v>42</v>
       </c>
-      <c r="AP46" s="38"/>
-      <c r="AQ46" s="37">
+      <c r="AP46" s="41"/>
+      <c r="AQ46" s="45">
         <v>8</v>
       </c>
-      <c r="AR46" s="39"/>
-      <c r="AS46" s="39">
+      <c r="AR46" s="40"/>
+      <c r="AS46" s="40">
         <v>22</v>
       </c>
-      <c r="AT46" s="39"/>
-      <c r="AU46" s="39">
+      <c r="AT46" s="40"/>
+      <c r="AU46" s="40">
         <v>26</v>
       </c>
-      <c r="AV46" s="38"/>
+      <c r="AV46" s="41"/>
       <c r="AW46" s="46" t="s">
         <v>10</v>
       </c>
+      <c r="BN46" s="45">
+        <v>42</v>
+      </c>
+      <c r="BO46" s="41"/>
+      <c r="BP46" s="45">
+        <v>8</v>
+      </c>
+      <c r="BQ46" s="40"/>
+      <c r="BR46" s="40">
+        <v>22</v>
+      </c>
+      <c r="BS46" s="40"/>
+      <c r="BT46" s="40">
+        <v>26</v>
+      </c>
+      <c r="BU46" s="41"/>
+      <c r="BV46" s="46" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="47" spans="3:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D47">
         <v>20</v>
       </c>
@@ -4020,25 +5186,42 @@
       <c r="AC47">
         <v>5</v>
       </c>
-      <c r="AO47" s="37">
+      <c r="AO47" s="45">
         <v>43</v>
       </c>
-      <c r="AP47" s="38"/>
-      <c r="AQ47" s="37">
+      <c r="AP47" s="41"/>
+      <c r="AQ47" s="45">
         <v>8</v>
       </c>
-      <c r="AR47" s="39"/>
-      <c r="AS47" s="39">
+      <c r="AR47" s="40"/>
+      <c r="AS47" s="40">
         <v>26</v>
       </c>
-      <c r="AT47" s="39"/>
-      <c r="AU47" s="39">
+      <c r="AT47" s="40"/>
+      <c r="AU47" s="40">
         <v>12</v>
       </c>
-      <c r="AV47" s="38"/>
+      <c r="AV47" s="41"/>
       <c r="AW47" s="47"/>
+      <c r="BN47" s="45">
+        <v>43</v>
+      </c>
+      <c r="BO47" s="41"/>
+      <c r="BP47" s="45">
+        <v>8</v>
+      </c>
+      <c r="BQ47" s="40"/>
+      <c r="BR47" s="40">
+        <v>26</v>
+      </c>
+      <c r="BS47" s="40"/>
+      <c r="BT47" s="40">
+        <v>12</v>
+      </c>
+      <c r="BU47" s="41"/>
+      <c r="BV47" s="47"/>
     </row>
-    <row r="48" spans="3:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D48">
         <v>14</v>
       </c>
@@ -4063,25 +5246,42 @@
       <c r="Y48">
         <v>11</v>
       </c>
-      <c r="AO48" s="37">
+      <c r="AO48" s="45">
         <v>44</v>
       </c>
-      <c r="AP48" s="38"/>
-      <c r="AQ48" s="37">
+      <c r="AP48" s="41"/>
+      <c r="AQ48" s="45">
         <v>13</v>
       </c>
-      <c r="AR48" s="39"/>
-      <c r="AS48" s="39">
+      <c r="AR48" s="40"/>
+      <c r="AS48" s="40">
         <v>12</v>
       </c>
-      <c r="AT48" s="39"/>
-      <c r="AU48" s="39">
+      <c r="AT48" s="40"/>
+      <c r="AU48" s="40">
         <v>26</v>
       </c>
-      <c r="AV48" s="38"/>
+      <c r="AV48" s="41"/>
       <c r="AW48" s="47"/>
+      <c r="BN48" s="45">
+        <v>44</v>
+      </c>
+      <c r="BO48" s="41"/>
+      <c r="BP48" s="45">
+        <v>13</v>
+      </c>
+      <c r="BQ48" s="40"/>
+      <c r="BR48" s="40">
+        <v>12</v>
+      </c>
+      <c r="BS48" s="40"/>
+      <c r="BT48" s="40">
+        <v>26</v>
+      </c>
+      <c r="BU48" s="41"/>
+      <c r="BV48" s="47"/>
     </row>
-    <row r="49" spans="4:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E49" s="3"/>
       <c r="F49" s="1"/>
       <c r="G49" s="33"/>
@@ -4102,25 +5302,42 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
       <c r="AC49" s="2"/>
-      <c r="AO49" s="37">
+      <c r="AO49" s="45">
         <v>45</v>
       </c>
-      <c r="AP49" s="38"/>
-      <c r="AQ49" s="37">
+      <c r="AP49" s="41"/>
+      <c r="AQ49" s="45">
         <v>13</v>
       </c>
-      <c r="AR49" s="39"/>
-      <c r="AS49" s="39">
+      <c r="AR49" s="40"/>
+      <c r="AS49" s="40">
         <v>26</v>
       </c>
-      <c r="AT49" s="39"/>
-      <c r="AU49" s="39">
+      <c r="AT49" s="40"/>
+      <c r="AU49" s="40">
         <v>27</v>
       </c>
-      <c r="AV49" s="38"/>
+      <c r="AV49" s="41"/>
       <c r="AW49" s="47"/>
+      <c r="BN49" s="45">
+        <v>45</v>
+      </c>
+      <c r="BO49" s="41"/>
+      <c r="BP49" s="45">
+        <v>13</v>
+      </c>
+      <c r="BQ49" s="40"/>
+      <c r="BR49" s="40">
+        <v>26</v>
+      </c>
+      <c r="BS49" s="40"/>
+      <c r="BT49" s="40">
+        <v>27</v>
+      </c>
+      <c r="BU49" s="41"/>
+      <c r="BV49" s="47"/>
     </row>
-    <row r="50" spans="4:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E50" s="9"/>
       <c r="F50" s="7"/>
       <c r="G50" s="35"/>
@@ -4141,25 +5358,42 @@
       <c r="AA50" s="7"/>
       <c r="AB50" s="7"/>
       <c r="AC50" s="8"/>
-      <c r="AO50" s="37">
+      <c r="AO50" s="45">
         <v>46</v>
       </c>
-      <c r="AP50" s="38"/>
-      <c r="AQ50" s="37">
+      <c r="AP50" s="41"/>
+      <c r="AQ50" s="45">
         <v>13</v>
       </c>
-      <c r="AR50" s="39"/>
-      <c r="AS50" s="39">
+      <c r="AR50" s="40"/>
+      <c r="AS50" s="40">
         <v>27</v>
       </c>
-      <c r="AT50" s="39"/>
-      <c r="AU50" s="39">
+      <c r="AT50" s="40"/>
+      <c r="AU50" s="40">
         <v>25</v>
       </c>
-      <c r="AV50" s="38"/>
+      <c r="AV50" s="41"/>
       <c r="AW50" s="47"/>
+      <c r="BN50" s="45">
+        <v>46</v>
+      </c>
+      <c r="BO50" s="41"/>
+      <c r="BP50" s="45">
+        <v>13</v>
+      </c>
+      <c r="BQ50" s="40"/>
+      <c r="BR50" s="40">
+        <v>27</v>
+      </c>
+      <c r="BS50" s="40"/>
+      <c r="BT50" s="40">
+        <v>25</v>
+      </c>
+      <c r="BU50" s="41"/>
+      <c r="BV50" s="47"/>
     </row>
-    <row r="51" spans="4:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D51">
         <v>0</v>
       </c>
@@ -4184,25 +5418,42 @@
       <c r="Y51">
         <v>25</v>
       </c>
-      <c r="AO51" s="37">
+      <c r="AO51" s="45">
         <v>47</v>
       </c>
-      <c r="AP51" s="38"/>
-      <c r="AQ51" s="37">
+      <c r="AP51" s="41"/>
+      <c r="AQ51" s="45">
         <v>13</v>
       </c>
-      <c r="AR51" s="39"/>
-      <c r="AS51" s="39">
+      <c r="AR51" s="40"/>
+      <c r="AS51" s="40">
         <v>25</v>
       </c>
-      <c r="AT51" s="39"/>
-      <c r="AU51" s="39">
+      <c r="AT51" s="40"/>
+      <c r="AU51" s="40">
         <v>11</v>
       </c>
-      <c r="AV51" s="38"/>
+      <c r="AV51" s="41"/>
       <c r="AW51" s="47"/>
+      <c r="BN51" s="45">
+        <v>47</v>
+      </c>
+      <c r="BO51" s="41"/>
+      <c r="BP51" s="45">
+        <v>13</v>
+      </c>
+      <c r="BQ51" s="40"/>
+      <c r="BR51" s="40">
+        <v>25</v>
+      </c>
+      <c r="BS51" s="40"/>
+      <c r="BT51" s="40">
+        <v>11</v>
+      </c>
+      <c r="BU51" s="41"/>
+      <c r="BV51" s="47"/>
     </row>
-    <row r="52" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D52">
         <v>6</v>
       </c>
@@ -4221,90 +5472,158 @@
       <c r="AC52">
         <v>19</v>
       </c>
-      <c r="AO52" s="37">
+      <c r="AO52" s="45">
         <v>48</v>
       </c>
-      <c r="AP52" s="38"/>
-      <c r="AQ52" s="37">
+      <c r="AP52" s="41"/>
+      <c r="AQ52" s="45">
         <v>4</v>
       </c>
-      <c r="AR52" s="39"/>
-      <c r="AS52" s="39">
+      <c r="AR52" s="40"/>
+      <c r="AS52" s="40">
         <v>18</v>
       </c>
-      <c r="AT52" s="39"/>
-      <c r="AU52" s="39">
+      <c r="AT52" s="40"/>
+      <c r="AU52" s="40">
         <v>19</v>
       </c>
-      <c r="AV52" s="38"/>
+      <c r="AV52" s="41"/>
       <c r="AW52" s="47"/>
+      <c r="BN52" s="45">
+        <v>48</v>
+      </c>
+      <c r="BO52" s="41"/>
+      <c r="BP52" s="45">
+        <v>4</v>
+      </c>
+      <c r="BQ52" s="40"/>
+      <c r="BR52" s="40">
+        <v>18</v>
+      </c>
+      <c r="BS52" s="40"/>
+      <c r="BT52" s="40">
+        <v>19</v>
+      </c>
+      <c r="BU52" s="41"/>
+      <c r="BV52" s="47"/>
     </row>
-    <row r="53" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AO53" s="37">
+    <row r="53" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AO53" s="45">
         <v>49</v>
       </c>
-      <c r="AP53" s="38"/>
-      <c r="AQ53" s="37">
+      <c r="AP53" s="41"/>
+      <c r="AQ53" s="45">
         <v>4</v>
       </c>
-      <c r="AR53" s="39"/>
-      <c r="AS53" s="39">
+      <c r="AR53" s="40"/>
+      <c r="AS53" s="40">
         <v>19</v>
       </c>
-      <c r="AT53" s="39"/>
-      <c r="AU53" s="39">
+      <c r="AT53" s="40"/>
+      <c r="AU53" s="40">
         <v>5</v>
       </c>
-      <c r="AV53" s="38"/>
+      <c r="AV53" s="41"/>
       <c r="AW53" s="47"/>
+      <c r="BN53" s="45">
+        <v>49</v>
+      </c>
+      <c r="BO53" s="41"/>
+      <c r="BP53" s="45">
+        <v>4</v>
+      </c>
+      <c r="BQ53" s="40"/>
+      <c r="BR53" s="40">
+        <v>19</v>
+      </c>
+      <c r="BS53" s="40"/>
+      <c r="BT53" s="40">
+        <v>5</v>
+      </c>
+      <c r="BU53" s="41"/>
+      <c r="BV53" s="47"/>
     </row>
-    <row r="54" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AO54" s="37">
+    <row r="54" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AO54" s="45">
         <v>50</v>
       </c>
-      <c r="AP54" s="38"/>
-      <c r="AQ54" s="37">
+      <c r="AP54" s="41"/>
+      <c r="AQ54" s="45">
         <v>3</v>
       </c>
-      <c r="AR54" s="39"/>
-      <c r="AS54" s="39">
+      <c r="AR54" s="40"/>
+      <c r="AS54" s="40">
         <v>2</v>
       </c>
-      <c r="AT54" s="39"/>
-      <c r="AU54" s="39">
+      <c r="AT54" s="40"/>
+      <c r="AU54" s="40">
         <v>16</v>
       </c>
-      <c r="AV54" s="38"/>
+      <c r="AV54" s="41"/>
       <c r="AW54" s="47"/>
+      <c r="BN54" s="45">
+        <v>50</v>
+      </c>
+      <c r="BO54" s="41"/>
+      <c r="BP54" s="45">
+        <v>3</v>
+      </c>
+      <c r="BQ54" s="40"/>
+      <c r="BR54" s="40">
+        <v>2</v>
+      </c>
+      <c r="BS54" s="40"/>
+      <c r="BT54" s="40">
+        <v>16</v>
+      </c>
+      <c r="BU54" s="41"/>
+      <c r="BV54" s="47"/>
     </row>
-    <row r="55" spans="4:49" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AO55" s="53">
+    <row r="55" spans="4:74" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AO55" s="44">
         <v>51</v>
       </c>
-      <c r="AP55" s="54"/>
-      <c r="AQ55" s="53">
+      <c r="AP55" s="43"/>
+      <c r="AQ55" s="44">
         <v>3</v>
       </c>
-      <c r="AR55" s="55"/>
-      <c r="AS55" s="55">
+      <c r="AR55" s="42"/>
+      <c r="AS55" s="42">
         <v>16</v>
       </c>
-      <c r="AT55" s="55"/>
-      <c r="AU55" s="55">
+      <c r="AT55" s="42"/>
+      <c r="AU55" s="42">
         <v>17</v>
       </c>
-      <c r="AV55" s="54"/>
+      <c r="AV55" s="43"/>
       <c r="AW55" s="48"/>
+      <c r="BN55" s="44">
+        <v>51</v>
+      </c>
+      <c r="BO55" s="43"/>
+      <c r="BP55" s="44">
+        <v>3</v>
+      </c>
+      <c r="BQ55" s="42"/>
+      <c r="BR55" s="42">
+        <v>16</v>
+      </c>
+      <c r="BS55" s="42"/>
+      <c r="BT55" s="42">
+        <v>17</v>
+      </c>
+      <c r="BU55" s="43"/>
+      <c r="BV55" s="48"/>
     </row>
-    <row r="56" spans="4:49" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="4:49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="4:74" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="4:74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4314,43 +5633,580 @@
     <row r="71" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="72" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="335">
-    <mergeCell ref="BB3:BI3"/>
-    <mergeCell ref="AU48:AV48"/>
-    <mergeCell ref="AU53:AV53"/>
-    <mergeCell ref="AU50:AV50"/>
-    <mergeCell ref="AU51:AV51"/>
-    <mergeCell ref="AU54:AV54"/>
-    <mergeCell ref="AU55:AV55"/>
-    <mergeCell ref="AU49:AV49"/>
-    <mergeCell ref="AU52:AV52"/>
-    <mergeCell ref="AS48:AT48"/>
-    <mergeCell ref="AS53:AT53"/>
-    <mergeCell ref="AS50:AT50"/>
-    <mergeCell ref="AS51:AT51"/>
-    <mergeCell ref="AS54:AT54"/>
-    <mergeCell ref="AS55:AT55"/>
-    <mergeCell ref="AS49:AT49"/>
-    <mergeCell ref="AS52:AT52"/>
-    <mergeCell ref="AO55:AP55"/>
-    <mergeCell ref="AQ48:AR48"/>
-    <mergeCell ref="AQ53:AR53"/>
-    <mergeCell ref="AQ50:AR50"/>
-    <mergeCell ref="AQ51:AR51"/>
-    <mergeCell ref="AQ54:AR54"/>
-    <mergeCell ref="AQ55:AR55"/>
-    <mergeCell ref="AO49:AP49"/>
-    <mergeCell ref="AQ49:AR49"/>
-    <mergeCell ref="AO52:AP52"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="AO48:AP48"/>
-    <mergeCell ref="AO53:AP53"/>
-    <mergeCell ref="AO50:AP50"/>
-    <mergeCell ref="AO51:AP51"/>
-    <mergeCell ref="AO54:AP54"/>
-    <mergeCell ref="W46:Z46"/>
-    <mergeCell ref="AO47:AP47"/>
-    <mergeCell ref="AQ47:AR47"/>
+  <mergeCells count="637">
+    <mergeCell ref="BN54:BO54"/>
+    <mergeCell ref="BP54:BQ54"/>
+    <mergeCell ref="BR54:BS54"/>
+    <mergeCell ref="BT54:BU54"/>
+    <mergeCell ref="BN55:BO55"/>
+    <mergeCell ref="BP55:BQ55"/>
+    <mergeCell ref="BR55:BS55"/>
+    <mergeCell ref="BT55:BU55"/>
+    <mergeCell ref="BT43:BU43"/>
+    <mergeCell ref="BT44:BU44"/>
+    <mergeCell ref="BT45:BU45"/>
+    <mergeCell ref="BT46:BU46"/>
+    <mergeCell ref="BV46:BV55"/>
+    <mergeCell ref="BT47:BU47"/>
+    <mergeCell ref="BT48:BU48"/>
+    <mergeCell ref="BT49:BU49"/>
+    <mergeCell ref="BT50:BU50"/>
+    <mergeCell ref="BT51:BU51"/>
+    <mergeCell ref="BT52:BU52"/>
+    <mergeCell ref="BT53:BU53"/>
+    <mergeCell ref="BT32:BU32"/>
+    <mergeCell ref="BV32:BV39"/>
+    <mergeCell ref="BT33:BU33"/>
+    <mergeCell ref="BT34:BU34"/>
+    <mergeCell ref="BT35:BU35"/>
+    <mergeCell ref="BT36:BU36"/>
+    <mergeCell ref="BT37:BU37"/>
+    <mergeCell ref="BT38:BU38"/>
+    <mergeCell ref="BT39:BU39"/>
+    <mergeCell ref="BR8:BS8"/>
+    <mergeCell ref="BN3:BU3"/>
+    <mergeCell ref="BT4:BU4"/>
+    <mergeCell ref="BV4:BV13"/>
+    <mergeCell ref="BT5:BU5"/>
+    <mergeCell ref="BT6:BU6"/>
+    <mergeCell ref="BT7:BU7"/>
+    <mergeCell ref="BT8:BU8"/>
+    <mergeCell ref="BT9:BU9"/>
+    <mergeCell ref="BT10:BU10"/>
+    <mergeCell ref="BT11:BU11"/>
+    <mergeCell ref="BT12:BU12"/>
+    <mergeCell ref="BT13:BU13"/>
+    <mergeCell ref="BT14:BU14"/>
+    <mergeCell ref="BV14:BV23"/>
+    <mergeCell ref="BT15:BU15"/>
+    <mergeCell ref="BT16:BU16"/>
+    <mergeCell ref="BT17:BU17"/>
+    <mergeCell ref="BP11:BQ11"/>
+    <mergeCell ref="BN11:BO11"/>
+    <mergeCell ref="BR10:BS10"/>
+    <mergeCell ref="BP10:BQ10"/>
+    <mergeCell ref="BN10:BO10"/>
+    <mergeCell ref="BR9:BS9"/>
+    <mergeCell ref="BP9:BQ9"/>
+    <mergeCell ref="BN9:BO9"/>
+    <mergeCell ref="BR11:BS11"/>
+    <mergeCell ref="BT18:BU18"/>
+    <mergeCell ref="BT19:BU19"/>
+    <mergeCell ref="BT20:BU20"/>
+    <mergeCell ref="BT21:BU21"/>
+    <mergeCell ref="BT22:BU22"/>
+    <mergeCell ref="BT23:BU23"/>
+    <mergeCell ref="BT24:BU24"/>
+    <mergeCell ref="BV24:BV31"/>
+    <mergeCell ref="BT25:BU25"/>
+    <mergeCell ref="BT26:BU26"/>
+    <mergeCell ref="BT27:BU27"/>
+    <mergeCell ref="BT28:BU28"/>
+    <mergeCell ref="BT29:BU29"/>
+    <mergeCell ref="BT30:BU30"/>
+    <mergeCell ref="BT31:BU31"/>
+    <mergeCell ref="BV40:BV45"/>
+    <mergeCell ref="BN52:BO52"/>
+    <mergeCell ref="BP52:BQ52"/>
+    <mergeCell ref="BR52:BS52"/>
+    <mergeCell ref="BN53:BO53"/>
+    <mergeCell ref="BP53:BQ53"/>
+    <mergeCell ref="BR53:BS53"/>
+    <mergeCell ref="BR49:BS49"/>
+    <mergeCell ref="BN50:BO50"/>
+    <mergeCell ref="BP50:BQ50"/>
+    <mergeCell ref="BR50:BS50"/>
+    <mergeCell ref="BN51:BO51"/>
+    <mergeCell ref="BP51:BQ51"/>
+    <mergeCell ref="BR51:BS51"/>
+    <mergeCell ref="BN44:BO44"/>
+    <mergeCell ref="BP44:BQ44"/>
+    <mergeCell ref="BR44:BS44"/>
+    <mergeCell ref="BN45:BO45"/>
+    <mergeCell ref="BP45:BQ45"/>
+    <mergeCell ref="BR45:BS45"/>
+    <mergeCell ref="BN46:BO46"/>
+    <mergeCell ref="BP46:BQ46"/>
+    <mergeCell ref="BR46:BS46"/>
+    <mergeCell ref="BN47:BO47"/>
+    <mergeCell ref="BP47:BQ47"/>
+    <mergeCell ref="BR47:BS47"/>
+    <mergeCell ref="BN48:BO48"/>
+    <mergeCell ref="BP48:BQ48"/>
+    <mergeCell ref="BR48:BS48"/>
+    <mergeCell ref="BN49:BO49"/>
+    <mergeCell ref="BP49:BQ49"/>
+    <mergeCell ref="BN39:BO39"/>
+    <mergeCell ref="BP39:BQ39"/>
+    <mergeCell ref="BR39:BS39"/>
+    <mergeCell ref="BN40:BO40"/>
+    <mergeCell ref="BP40:BQ40"/>
+    <mergeCell ref="BR40:BS40"/>
+    <mergeCell ref="BN41:BO41"/>
+    <mergeCell ref="BP41:BQ41"/>
+    <mergeCell ref="BR41:BS41"/>
+    <mergeCell ref="BN42:BO42"/>
+    <mergeCell ref="BP42:BQ42"/>
+    <mergeCell ref="BR42:BS42"/>
+    <mergeCell ref="BN43:BO43"/>
+    <mergeCell ref="BP43:BQ43"/>
+    <mergeCell ref="BR43:BS43"/>
+    <mergeCell ref="BT40:BU40"/>
+    <mergeCell ref="BT41:BU41"/>
+    <mergeCell ref="BT42:BU42"/>
+    <mergeCell ref="BR36:BS36"/>
+    <mergeCell ref="BN37:BO37"/>
+    <mergeCell ref="BP37:BQ37"/>
+    <mergeCell ref="BR37:BS37"/>
+    <mergeCell ref="BN38:BO38"/>
+    <mergeCell ref="BP38:BQ38"/>
+    <mergeCell ref="BR38:BS38"/>
+    <mergeCell ref="BN31:BO31"/>
+    <mergeCell ref="BP31:BQ31"/>
+    <mergeCell ref="BR31:BS31"/>
+    <mergeCell ref="BN32:BO32"/>
+    <mergeCell ref="BP32:BQ32"/>
+    <mergeCell ref="BR32:BS32"/>
+    <mergeCell ref="BN33:BO33"/>
+    <mergeCell ref="BP33:BQ33"/>
+    <mergeCell ref="BR33:BS33"/>
+    <mergeCell ref="BN34:BO34"/>
+    <mergeCell ref="BP34:BQ34"/>
+    <mergeCell ref="BR34:BS34"/>
+    <mergeCell ref="BN35:BO35"/>
+    <mergeCell ref="BP35:BQ35"/>
+    <mergeCell ref="BR35:BS35"/>
+    <mergeCell ref="BN36:BO36"/>
+    <mergeCell ref="BP36:BQ36"/>
+    <mergeCell ref="BR28:BS28"/>
+    <mergeCell ref="BN29:BO29"/>
+    <mergeCell ref="BP29:BQ29"/>
+    <mergeCell ref="BR29:BS29"/>
+    <mergeCell ref="BN30:BO30"/>
+    <mergeCell ref="BP30:BQ30"/>
+    <mergeCell ref="BR30:BS30"/>
+    <mergeCell ref="BN23:BO23"/>
+    <mergeCell ref="BP23:BQ23"/>
+    <mergeCell ref="BR23:BS23"/>
+    <mergeCell ref="BN24:BO24"/>
+    <mergeCell ref="BP24:BQ24"/>
+    <mergeCell ref="BR24:BS24"/>
+    <mergeCell ref="BN25:BO25"/>
+    <mergeCell ref="BP25:BQ25"/>
+    <mergeCell ref="BR25:BS25"/>
+    <mergeCell ref="BN26:BO26"/>
+    <mergeCell ref="BP26:BQ26"/>
+    <mergeCell ref="BR26:BS26"/>
+    <mergeCell ref="BN27:BO27"/>
+    <mergeCell ref="BP27:BQ27"/>
+    <mergeCell ref="BR27:BS27"/>
+    <mergeCell ref="BN28:BO28"/>
+    <mergeCell ref="BP28:BQ28"/>
+    <mergeCell ref="BN20:BO20"/>
+    <mergeCell ref="BP20:BQ20"/>
+    <mergeCell ref="BR20:BS20"/>
+    <mergeCell ref="BN21:BO21"/>
+    <mergeCell ref="BP21:BQ21"/>
+    <mergeCell ref="BR21:BS21"/>
+    <mergeCell ref="BN22:BO22"/>
+    <mergeCell ref="BP22:BQ22"/>
+    <mergeCell ref="BR22:BS22"/>
+    <mergeCell ref="BR17:BS17"/>
+    <mergeCell ref="BN18:BO18"/>
+    <mergeCell ref="BP18:BQ18"/>
+    <mergeCell ref="BR18:BS18"/>
+    <mergeCell ref="BN19:BO19"/>
+    <mergeCell ref="BP19:BQ19"/>
+    <mergeCell ref="BR19:BS19"/>
+    <mergeCell ref="BN12:BO12"/>
+    <mergeCell ref="BP12:BQ12"/>
+    <mergeCell ref="BR12:BS12"/>
+    <mergeCell ref="BN13:BO13"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="BR13:BS13"/>
+    <mergeCell ref="BN14:BO14"/>
+    <mergeCell ref="BP14:BQ14"/>
+    <mergeCell ref="BR14:BS14"/>
+    <mergeCell ref="BN15:BO15"/>
+    <mergeCell ref="BP15:BQ15"/>
+    <mergeCell ref="BR15:BS15"/>
+    <mergeCell ref="BN16:BO16"/>
+    <mergeCell ref="BP16:BQ16"/>
+    <mergeCell ref="BR16:BS16"/>
+    <mergeCell ref="BN17:BO17"/>
+    <mergeCell ref="BP17:BQ17"/>
+    <mergeCell ref="BN4:BO4"/>
+    <mergeCell ref="BP4:BQ4"/>
+    <mergeCell ref="BR4:BS4"/>
+    <mergeCell ref="BN5:BO5"/>
+    <mergeCell ref="BP5:BQ5"/>
+    <mergeCell ref="BR5:BS5"/>
+    <mergeCell ref="BN6:BO6"/>
+    <mergeCell ref="BP6:BQ6"/>
+    <mergeCell ref="BR6:BS6"/>
+    <mergeCell ref="BN7:BO7"/>
+    <mergeCell ref="BP7:BQ7"/>
+    <mergeCell ref="BR7:BS7"/>
+    <mergeCell ref="BN8:BO8"/>
+    <mergeCell ref="BP8:BQ8"/>
+    <mergeCell ref="BD30:BF30"/>
+    <mergeCell ref="BG30:BI30"/>
+    <mergeCell ref="BD31:BF31"/>
+    <mergeCell ref="BG31:BI31"/>
+    <mergeCell ref="BD32:BF32"/>
+    <mergeCell ref="BG32:BI32"/>
+    <mergeCell ref="BD25:BF25"/>
+    <mergeCell ref="BG25:BI25"/>
+    <mergeCell ref="BD26:BF26"/>
+    <mergeCell ref="BG26:BI26"/>
+    <mergeCell ref="BD27:BF27"/>
+    <mergeCell ref="BG27:BI27"/>
+    <mergeCell ref="BD28:BF28"/>
+    <mergeCell ref="BG28:BI28"/>
+    <mergeCell ref="BD29:BF29"/>
+    <mergeCell ref="BG29:BI29"/>
+    <mergeCell ref="BD20:BF20"/>
+    <mergeCell ref="BG20:BI20"/>
+    <mergeCell ref="BD21:BF21"/>
+    <mergeCell ref="BG21:BI21"/>
+    <mergeCell ref="BD22:BF22"/>
+    <mergeCell ref="BG22:BI22"/>
+    <mergeCell ref="BD23:BF23"/>
+    <mergeCell ref="BG23:BI23"/>
+    <mergeCell ref="BD24:BF24"/>
+    <mergeCell ref="BG24:BI24"/>
+    <mergeCell ref="BD15:BF15"/>
+    <mergeCell ref="BG15:BI15"/>
+    <mergeCell ref="BD16:BF16"/>
+    <mergeCell ref="BG16:BI16"/>
+    <mergeCell ref="BD17:BF17"/>
+    <mergeCell ref="BG17:BI17"/>
+    <mergeCell ref="BD18:BF18"/>
+    <mergeCell ref="BG18:BI18"/>
+    <mergeCell ref="BD19:BF19"/>
+    <mergeCell ref="BG19:BI19"/>
+    <mergeCell ref="BB32:BC32"/>
+    <mergeCell ref="BD5:BF5"/>
+    <mergeCell ref="BG5:BI5"/>
+    <mergeCell ref="BD6:BF6"/>
+    <mergeCell ref="BD7:BF7"/>
+    <mergeCell ref="BD8:BF8"/>
+    <mergeCell ref="BD9:BF9"/>
+    <mergeCell ref="BD10:BF10"/>
+    <mergeCell ref="BD11:BF11"/>
+    <mergeCell ref="BD12:BF12"/>
+    <mergeCell ref="BG6:BI6"/>
+    <mergeCell ref="BG7:BI7"/>
+    <mergeCell ref="BG8:BI8"/>
+    <mergeCell ref="BG9:BI9"/>
+    <mergeCell ref="BG10:BI10"/>
+    <mergeCell ref="BG11:BI11"/>
+    <mergeCell ref="BG12:BI12"/>
+    <mergeCell ref="BD13:BF13"/>
+    <mergeCell ref="BG13:BI13"/>
+    <mergeCell ref="BD14:BF14"/>
+    <mergeCell ref="BG14:BI14"/>
+    <mergeCell ref="BB31:BC31"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BB28:BC28"/>
+    <mergeCell ref="BB29:BC29"/>
+    <mergeCell ref="BB30:BC30"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="BB26:BC26"/>
+    <mergeCell ref="BB27:BC27"/>
+    <mergeCell ref="BB22:BC22"/>
+    <mergeCell ref="BB23:BC23"/>
+    <mergeCell ref="BB24:BC24"/>
+    <mergeCell ref="BB19:BC19"/>
+    <mergeCell ref="BB20:BC20"/>
+    <mergeCell ref="BB21:BC21"/>
+    <mergeCell ref="BB16:BC16"/>
+    <mergeCell ref="BB17:BC17"/>
+    <mergeCell ref="BB18:BC18"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="BB14:BC14"/>
+    <mergeCell ref="BB15:BC15"/>
+    <mergeCell ref="BB10:BC10"/>
+    <mergeCell ref="BB11:BC11"/>
+    <mergeCell ref="BB12:BC12"/>
+    <mergeCell ref="BB8:BC8"/>
+    <mergeCell ref="BB9:BC9"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AG8:AH8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="AE13:AF13"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="AC3:AJ3"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AE19:AF19"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AE16:AF16"/>
+    <mergeCell ref="AG16:AH16"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AE17:AF17"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AI14:AJ14"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AI16:AJ16"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AI19:AJ19"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AI9:AJ9"/>
+    <mergeCell ref="AI10:AJ10"/>
+    <mergeCell ref="AI11:AJ11"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="AI13:AJ13"/>
+    <mergeCell ref="AI20:AJ20"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AE22:AF22"/>
+    <mergeCell ref="AG22:AH22"/>
+    <mergeCell ref="AI22:AJ22"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="AI21:AJ21"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AE20:AF20"/>
+    <mergeCell ref="AG20:AH20"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AO3:AV3"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="AQ10:AR10"/>
+    <mergeCell ref="AS10:AT10"/>
+    <mergeCell ref="AU10:AV10"/>
+    <mergeCell ref="AO11:AP11"/>
+    <mergeCell ref="AQ11:AR11"/>
+    <mergeCell ref="AS11:AT11"/>
+    <mergeCell ref="AU11:AV11"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AO9:AP9"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AU9:AV9"/>
+    <mergeCell ref="AO14:AP14"/>
+    <mergeCell ref="AQ14:AR14"/>
+    <mergeCell ref="AS14:AT14"/>
+    <mergeCell ref="AU14:AV14"/>
+    <mergeCell ref="AO15:AP15"/>
+    <mergeCell ref="AQ15:AR15"/>
+    <mergeCell ref="AS15:AT15"/>
+    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="AO12:AP12"/>
+    <mergeCell ref="AQ12:AR12"/>
+    <mergeCell ref="AS12:AT12"/>
+    <mergeCell ref="AU12:AV12"/>
+    <mergeCell ref="AO13:AP13"/>
+    <mergeCell ref="AQ13:AR13"/>
+    <mergeCell ref="AS13:AT13"/>
+    <mergeCell ref="AU13:AV13"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AQ18:AR18"/>
+    <mergeCell ref="AS18:AT18"/>
+    <mergeCell ref="AU18:AV18"/>
+    <mergeCell ref="AO19:AP19"/>
+    <mergeCell ref="AQ19:AR19"/>
+    <mergeCell ref="AS19:AT19"/>
+    <mergeCell ref="AU19:AV19"/>
+    <mergeCell ref="AO16:AP16"/>
+    <mergeCell ref="AQ16:AR16"/>
+    <mergeCell ref="AS16:AT16"/>
+    <mergeCell ref="AU16:AV16"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AQ17:AR17"/>
+    <mergeCell ref="AS17:AT17"/>
+    <mergeCell ref="AU17:AV17"/>
+    <mergeCell ref="AC25:AD25"/>
+    <mergeCell ref="AE25:AF25"/>
+    <mergeCell ref="AG25:AH25"/>
+    <mergeCell ref="AI25:AJ25"/>
+    <mergeCell ref="AO23:AP23"/>
+    <mergeCell ref="AQ23:AR23"/>
+    <mergeCell ref="AS23:AT23"/>
+    <mergeCell ref="AU23:AV23"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AO25:AP25"/>
+    <mergeCell ref="AQ25:AR25"/>
+    <mergeCell ref="AS25:AT25"/>
+    <mergeCell ref="AU25:AV25"/>
+    <mergeCell ref="AG29:AH29"/>
+    <mergeCell ref="AI29:AJ29"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AI26:AJ26"/>
+    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AE27:AF27"/>
+    <mergeCell ref="AG27:AH27"/>
+    <mergeCell ref="AI27:AJ27"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="AW4:AW13"/>
+    <mergeCell ref="AW14:AW23"/>
+    <mergeCell ref="AO24:AP24"/>
+    <mergeCell ref="AQ24:AR24"/>
+    <mergeCell ref="AS24:AT24"/>
+    <mergeCell ref="AU24:AV24"/>
+    <mergeCell ref="AS21:AT21"/>
+    <mergeCell ref="AU21:AV21"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="AS22:AT22"/>
+    <mergeCell ref="AU22:AV22"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="AG24:AH24"/>
+    <mergeCell ref="AI24:AJ24"/>
+    <mergeCell ref="AO20:AP20"/>
+    <mergeCell ref="AQ20:AR20"/>
+    <mergeCell ref="AS20:AT20"/>
+    <mergeCell ref="AU20:AV20"/>
+    <mergeCell ref="AO21:AP21"/>
+    <mergeCell ref="AQ21:AR21"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AQ26:AR26"/>
+    <mergeCell ref="AS26:AT26"/>
+    <mergeCell ref="AU26:AV26"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="AC30:AD30"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AE30:AF30"/>
+    <mergeCell ref="AG30:AH30"/>
+    <mergeCell ref="AI30:AJ30"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AG31:AH31"/>
+    <mergeCell ref="AI31:AJ31"/>
+    <mergeCell ref="AC28:AD28"/>
+    <mergeCell ref="AE28:AF28"/>
+    <mergeCell ref="AG28:AH28"/>
+    <mergeCell ref="AI28:AJ28"/>
+    <mergeCell ref="AC29:AD29"/>
+    <mergeCell ref="AE29:AF29"/>
+    <mergeCell ref="AO29:AP29"/>
+    <mergeCell ref="AQ29:AR29"/>
+    <mergeCell ref="AS29:AT29"/>
+    <mergeCell ref="AU29:AV29"/>
+    <mergeCell ref="AO30:AP30"/>
+    <mergeCell ref="AQ30:AR30"/>
+    <mergeCell ref="AS30:AT30"/>
+    <mergeCell ref="AU30:AV30"/>
+    <mergeCell ref="AO27:AP27"/>
+    <mergeCell ref="AQ27:AR27"/>
+    <mergeCell ref="AS27:AT27"/>
+    <mergeCell ref="AU27:AV27"/>
+    <mergeCell ref="AO28:AP28"/>
+    <mergeCell ref="AQ28:AR28"/>
+    <mergeCell ref="AS28:AT28"/>
+    <mergeCell ref="AU28:AV28"/>
+    <mergeCell ref="AO33:AP33"/>
+    <mergeCell ref="AQ33:AR33"/>
+    <mergeCell ref="AS33:AT33"/>
+    <mergeCell ref="AU33:AV33"/>
+    <mergeCell ref="AO34:AP34"/>
+    <mergeCell ref="AQ34:AR34"/>
+    <mergeCell ref="AS34:AT34"/>
+    <mergeCell ref="AU34:AV34"/>
+    <mergeCell ref="AO31:AP31"/>
+    <mergeCell ref="AQ31:AR31"/>
+    <mergeCell ref="AS31:AT31"/>
+    <mergeCell ref="AU31:AV31"/>
+    <mergeCell ref="AO32:AP32"/>
+    <mergeCell ref="AQ32:AR32"/>
+    <mergeCell ref="AS32:AT32"/>
+    <mergeCell ref="AU32:AV32"/>
+    <mergeCell ref="AO37:AP37"/>
+    <mergeCell ref="AQ37:AR37"/>
+    <mergeCell ref="AS37:AT37"/>
+    <mergeCell ref="AU37:AV37"/>
+    <mergeCell ref="AO38:AP38"/>
+    <mergeCell ref="AQ38:AR38"/>
+    <mergeCell ref="AS38:AT38"/>
+    <mergeCell ref="AU38:AV38"/>
+    <mergeCell ref="AO35:AP35"/>
+    <mergeCell ref="AQ35:AR35"/>
+    <mergeCell ref="AS35:AT35"/>
+    <mergeCell ref="AU35:AV35"/>
+    <mergeCell ref="AO36:AP36"/>
+    <mergeCell ref="AQ36:AR36"/>
+    <mergeCell ref="AS36:AT36"/>
+    <mergeCell ref="AU36:AV36"/>
+    <mergeCell ref="AQ41:AR41"/>
+    <mergeCell ref="AS41:AT41"/>
+    <mergeCell ref="AU41:AV41"/>
+    <mergeCell ref="AO42:AP42"/>
+    <mergeCell ref="AQ42:AR42"/>
+    <mergeCell ref="AS42:AT42"/>
+    <mergeCell ref="AU42:AV42"/>
+    <mergeCell ref="AO39:AP39"/>
+    <mergeCell ref="AQ39:AR39"/>
+    <mergeCell ref="AS39:AT39"/>
+    <mergeCell ref="AU39:AV39"/>
+    <mergeCell ref="AO40:AP40"/>
+    <mergeCell ref="AQ40:AR40"/>
+    <mergeCell ref="AS40:AT40"/>
+    <mergeCell ref="AU40:AV40"/>
     <mergeCell ref="AS47:AT47"/>
     <mergeCell ref="AU47:AV47"/>
     <mergeCell ref="AW32:AW39"/>
@@ -4375,281 +6231,46 @@
     <mergeCell ref="AS44:AT44"/>
     <mergeCell ref="AU44:AV44"/>
     <mergeCell ref="AO41:AP41"/>
-    <mergeCell ref="AQ41:AR41"/>
-    <mergeCell ref="AS41:AT41"/>
-    <mergeCell ref="AU41:AV41"/>
-    <mergeCell ref="AO42:AP42"/>
-    <mergeCell ref="AQ42:AR42"/>
-    <mergeCell ref="AS42:AT42"/>
-    <mergeCell ref="AU42:AV42"/>
-    <mergeCell ref="AO39:AP39"/>
-    <mergeCell ref="AQ39:AR39"/>
-    <mergeCell ref="AS39:AT39"/>
-    <mergeCell ref="AU39:AV39"/>
-    <mergeCell ref="AO40:AP40"/>
-    <mergeCell ref="AQ40:AR40"/>
-    <mergeCell ref="AS40:AT40"/>
-    <mergeCell ref="AU40:AV40"/>
-    <mergeCell ref="AO37:AP37"/>
-    <mergeCell ref="AQ37:AR37"/>
-    <mergeCell ref="AS37:AT37"/>
-    <mergeCell ref="AU37:AV37"/>
-    <mergeCell ref="AO38:AP38"/>
-    <mergeCell ref="AQ38:AR38"/>
-    <mergeCell ref="AS38:AT38"/>
-    <mergeCell ref="AU38:AV38"/>
-    <mergeCell ref="AO35:AP35"/>
-    <mergeCell ref="AQ35:AR35"/>
-    <mergeCell ref="AS35:AT35"/>
-    <mergeCell ref="AU35:AV35"/>
-    <mergeCell ref="AO36:AP36"/>
-    <mergeCell ref="AQ36:AR36"/>
-    <mergeCell ref="AS36:AT36"/>
-    <mergeCell ref="AU36:AV36"/>
-    <mergeCell ref="AO33:AP33"/>
-    <mergeCell ref="AQ33:AR33"/>
-    <mergeCell ref="AS33:AT33"/>
-    <mergeCell ref="AU33:AV33"/>
-    <mergeCell ref="AO34:AP34"/>
-    <mergeCell ref="AQ34:AR34"/>
-    <mergeCell ref="AS34:AT34"/>
-    <mergeCell ref="AU34:AV34"/>
-    <mergeCell ref="AO31:AP31"/>
-    <mergeCell ref="AQ31:AR31"/>
-    <mergeCell ref="AS31:AT31"/>
-    <mergeCell ref="AU31:AV31"/>
-    <mergeCell ref="AO32:AP32"/>
-    <mergeCell ref="AQ32:AR32"/>
-    <mergeCell ref="AS32:AT32"/>
-    <mergeCell ref="AU32:AV32"/>
-    <mergeCell ref="AO30:AP30"/>
-    <mergeCell ref="AQ30:AR30"/>
-    <mergeCell ref="AS30:AT30"/>
-    <mergeCell ref="AU30:AV30"/>
-    <mergeCell ref="AO27:AP27"/>
-    <mergeCell ref="AQ27:AR27"/>
-    <mergeCell ref="AS27:AT27"/>
-    <mergeCell ref="AU27:AV27"/>
-    <mergeCell ref="AO28:AP28"/>
-    <mergeCell ref="AQ28:AR28"/>
-    <mergeCell ref="AS28:AT28"/>
-    <mergeCell ref="AU28:AV28"/>
-    <mergeCell ref="AO26:AP26"/>
-    <mergeCell ref="AQ26:AR26"/>
-    <mergeCell ref="AS26:AT26"/>
-    <mergeCell ref="AU26:AV26"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="AC30:AD30"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AE30:AF30"/>
-    <mergeCell ref="AG30:AH30"/>
-    <mergeCell ref="AI30:AJ30"/>
-    <mergeCell ref="AE31:AF31"/>
-    <mergeCell ref="AG31:AH31"/>
-    <mergeCell ref="AI31:AJ31"/>
-    <mergeCell ref="AC28:AD28"/>
-    <mergeCell ref="AE28:AF28"/>
-    <mergeCell ref="AG28:AH28"/>
-    <mergeCell ref="AI28:AJ28"/>
-    <mergeCell ref="AC29:AD29"/>
-    <mergeCell ref="AE29:AF29"/>
-    <mergeCell ref="AO29:AP29"/>
-    <mergeCell ref="AQ29:AR29"/>
-    <mergeCell ref="AS29:AT29"/>
-    <mergeCell ref="AU29:AV29"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="AW4:AW13"/>
-    <mergeCell ref="AW14:AW23"/>
-    <mergeCell ref="AO24:AP24"/>
-    <mergeCell ref="AQ24:AR24"/>
-    <mergeCell ref="AS24:AT24"/>
-    <mergeCell ref="AU24:AV24"/>
-    <mergeCell ref="AS21:AT21"/>
-    <mergeCell ref="AU21:AV21"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="AS22:AT22"/>
-    <mergeCell ref="AU22:AV22"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AI24:AJ24"/>
-    <mergeCell ref="AO20:AP20"/>
-    <mergeCell ref="AQ20:AR20"/>
-    <mergeCell ref="AS20:AT20"/>
-    <mergeCell ref="AU20:AV20"/>
-    <mergeCell ref="AO21:AP21"/>
-    <mergeCell ref="AQ21:AR21"/>
-    <mergeCell ref="AG29:AH29"/>
-    <mergeCell ref="AI29:AJ29"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AI26:AJ26"/>
-    <mergeCell ref="AC27:AD27"/>
-    <mergeCell ref="AE27:AF27"/>
-    <mergeCell ref="AG27:AH27"/>
-    <mergeCell ref="AI27:AJ27"/>
-    <mergeCell ref="AC25:AD25"/>
-    <mergeCell ref="AE25:AF25"/>
-    <mergeCell ref="AG25:AH25"/>
-    <mergeCell ref="AI25:AJ25"/>
-    <mergeCell ref="AO23:AP23"/>
-    <mergeCell ref="AQ23:AR23"/>
-    <mergeCell ref="AS23:AT23"/>
-    <mergeCell ref="AU23:AV23"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AO25:AP25"/>
-    <mergeCell ref="AQ25:AR25"/>
-    <mergeCell ref="AS25:AT25"/>
-    <mergeCell ref="AU25:AV25"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AQ18:AR18"/>
-    <mergeCell ref="AS18:AT18"/>
-    <mergeCell ref="AU18:AV18"/>
-    <mergeCell ref="AO19:AP19"/>
-    <mergeCell ref="AQ19:AR19"/>
-    <mergeCell ref="AS19:AT19"/>
-    <mergeCell ref="AU19:AV19"/>
-    <mergeCell ref="AO16:AP16"/>
-    <mergeCell ref="AQ16:AR16"/>
-    <mergeCell ref="AS16:AT16"/>
-    <mergeCell ref="AU16:AV16"/>
-    <mergeCell ref="AO17:AP17"/>
-    <mergeCell ref="AQ17:AR17"/>
-    <mergeCell ref="AS17:AT17"/>
-    <mergeCell ref="AU17:AV17"/>
-    <mergeCell ref="AO14:AP14"/>
-    <mergeCell ref="AQ14:AR14"/>
-    <mergeCell ref="AS14:AT14"/>
-    <mergeCell ref="AU14:AV14"/>
-    <mergeCell ref="AO15:AP15"/>
-    <mergeCell ref="AQ15:AR15"/>
-    <mergeCell ref="AS15:AT15"/>
-    <mergeCell ref="AU15:AV15"/>
-    <mergeCell ref="AO12:AP12"/>
-    <mergeCell ref="AQ12:AR12"/>
-    <mergeCell ref="AS12:AT12"/>
-    <mergeCell ref="AU12:AV12"/>
-    <mergeCell ref="AO13:AP13"/>
-    <mergeCell ref="AQ13:AR13"/>
-    <mergeCell ref="AS13:AT13"/>
-    <mergeCell ref="AU13:AV13"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="AQ10:AR10"/>
-    <mergeCell ref="AS10:AT10"/>
-    <mergeCell ref="AU10:AV10"/>
-    <mergeCell ref="AO11:AP11"/>
-    <mergeCell ref="AQ11:AR11"/>
-    <mergeCell ref="AS11:AT11"/>
-    <mergeCell ref="AU11:AV11"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AU9:AV9"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AO3:AV3"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AI20:AJ20"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AE22:AF22"/>
-    <mergeCell ref="AG22:AH22"/>
-    <mergeCell ref="AI22:AJ22"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="AE21:AF21"/>
-    <mergeCell ref="AG21:AH21"/>
-    <mergeCell ref="AI21:AJ21"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AE20:AF20"/>
-    <mergeCell ref="AG20:AH20"/>
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AI16:AJ16"/>
-    <mergeCell ref="AI17:AJ17"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AI19:AJ19"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AI9:AJ9"/>
-    <mergeCell ref="AI10:AJ10"/>
-    <mergeCell ref="AI11:AJ11"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="AI13:AJ13"/>
-    <mergeCell ref="AC3:AJ3"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="AG18:AH18"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AE19:AF19"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AE16:AF16"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AE17:AF17"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="AE13:AF13"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="AG11:AH11"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AG8:AH8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="AO48:AP48"/>
+    <mergeCell ref="AO53:AP53"/>
+    <mergeCell ref="AO50:AP50"/>
+    <mergeCell ref="AO51:AP51"/>
+    <mergeCell ref="AO54:AP54"/>
+    <mergeCell ref="W46:Z46"/>
+    <mergeCell ref="AO47:AP47"/>
+    <mergeCell ref="AQ47:AR47"/>
+    <mergeCell ref="AS48:AT48"/>
+    <mergeCell ref="AS53:AT53"/>
+    <mergeCell ref="AS50:AT50"/>
+    <mergeCell ref="AS51:AT51"/>
+    <mergeCell ref="AS54:AT54"/>
+    <mergeCell ref="AS55:AT55"/>
+    <mergeCell ref="AS49:AT49"/>
+    <mergeCell ref="AS52:AT52"/>
+    <mergeCell ref="AO55:AP55"/>
+    <mergeCell ref="AQ48:AR48"/>
+    <mergeCell ref="AQ53:AR53"/>
+    <mergeCell ref="AQ50:AR50"/>
+    <mergeCell ref="AQ51:AR51"/>
+    <mergeCell ref="AQ54:AR54"/>
+    <mergeCell ref="AQ55:AR55"/>
+    <mergeCell ref="AO49:AP49"/>
+    <mergeCell ref="AQ49:AR49"/>
+    <mergeCell ref="AO52:AP52"/>
+    <mergeCell ref="BB3:BI3"/>
+    <mergeCell ref="AU48:AV48"/>
+    <mergeCell ref="AU53:AV53"/>
+    <mergeCell ref="AU50:AV50"/>
+    <mergeCell ref="AU51:AV51"/>
+    <mergeCell ref="AU54:AV54"/>
+    <mergeCell ref="AU55:AV55"/>
+    <mergeCell ref="AU49:AV49"/>
+    <mergeCell ref="AU52:AV52"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="BB5:BC5"/>
+    <mergeCell ref="BB6:BC6"/>
+    <mergeCell ref="BB7:BC7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>